<commit_message>
Laborator 30.11.2023 - CleanCode
</commit_message>
<xml_diff>
--- a/MetodeAvansate/Prezenta.xlsx
+++ b/MetodeAvansate/Prezenta.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\remus\Documents\GitHub\Facultate_2023\MetodeAvansate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D3645AF-6FE7-4263-9AA3-EF5B11C5CE90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13B8DB4F-96FE-4BD6-B8E2-8C49A9C20BB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="63">
   <si>
     <t>Nume Prenume</t>
   </si>
@@ -206,6 +206,9 @@
   </si>
   <si>
     <t>Tigan Andreea</t>
+  </si>
+  <si>
+    <t>Pecherle George</t>
   </si>
 </sst>
 </file>
@@ -399,7 +402,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -442,7 +445,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -726,10 +728,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:S46"/>
+  <dimension ref="B2:S47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="J53" sqref="J53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
@@ -822,7 +824,7 @@
       <c r="O3" s="4"/>
       <c r="P3" s="8"/>
       <c r="Q3" s="11">
-        <f t="shared" ref="Q3:Q45" si="0">C3+D3+E3+F3+G3+H3+I3+J3+K3+L3+M3+N3+O3+P3</f>
+        <f t="shared" ref="Q3:Q36" si="0">C3+D3+E3+F3+G3+H3+I3+J3+K3+L3+M3+N3+O3+P3</f>
         <v>4</v>
       </c>
       <c r="R3" s="12"/>
@@ -886,10 +888,13 @@
       <c r="J6" t="b">
         <v>1</v>
       </c>
+      <c r="K6" t="b">
+        <v>1</v>
+      </c>
       <c r="P6" s="9"/>
       <c r="Q6" s="11">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="R6" s="14"/>
       <c r="S6" s="15"/>
@@ -911,10 +916,13 @@
       <c r="J7" t="b">
         <v>1</v>
       </c>
+      <c r="K7" t="b">
+        <v>1</v>
+      </c>
       <c r="P7" s="9"/>
       <c r="Q7" s="11">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="R7" s="14"/>
       <c r="S7" s="15"/>
@@ -989,10 +997,13 @@
       <c r="J10" t="b">
         <v>1</v>
       </c>
+      <c r="K10" t="b">
+        <v>1</v>
+      </c>
       <c r="P10" s="9"/>
       <c r="Q10" s="11">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="R10" s="14"/>
       <c r="S10" s="15"/>
@@ -1005,10 +1016,13 @@
       <c r="J11" t="b">
         <v>1</v>
       </c>
+      <c r="K11" t="b">
+        <v>1</v>
+      </c>
       <c r="P11" s="9"/>
       <c r="Q11" s="11">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R11" s="14"/>
       <c r="S11" s="15"/>
@@ -1156,10 +1170,13 @@
       <c r="J17" t="b">
         <v>1</v>
       </c>
+      <c r="K17" t="b">
+        <v>1</v>
+      </c>
       <c r="P17" s="9"/>
       <c r="Q17" s="11">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="R17" s="14"/>
       <c r="S17" s="15"/>
@@ -1192,10 +1209,13 @@
       <c r="J18" t="b">
         <v>1</v>
       </c>
+      <c r="K18" t="b">
+        <v>1</v>
+      </c>
       <c r="P18" s="9"/>
       <c r="Q18" s="11">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="R18" s="14"/>
       <c r="S18" s="15"/>
@@ -1222,10 +1242,13 @@
       <c r="J19" t="b">
         <v>1</v>
       </c>
+      <c r="K19" t="b">
+        <v>1</v>
+      </c>
       <c r="P19" s="9"/>
       <c r="Q19" s="11">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="R19" s="14"/>
       <c r="S19" s="15"/>
@@ -1274,10 +1297,13 @@
       <c r="I21" t="b">
         <v>1</v>
       </c>
+      <c r="K21" t="b">
+        <v>1</v>
+      </c>
       <c r="P21" s="9"/>
       <c r="Q21" s="11">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="R21" s="14"/>
       <c r="S21" s="15"/>
@@ -1326,10 +1352,13 @@
       <c r="H23" t="b">
         <v>1</v>
       </c>
+      <c r="K23" t="b">
+        <v>1</v>
+      </c>
       <c r="P23" s="9"/>
       <c r="Q23" s="11">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="R23" s="14"/>
       <c r="S23" s="15"/>
@@ -1448,10 +1477,13 @@
       <c r="J28" t="b">
         <v>1</v>
       </c>
+      <c r="K28" t="b">
+        <v>1</v>
+      </c>
       <c r="P28" s="9"/>
       <c r="Q28" s="11">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="R28" s="14"/>
       <c r="S28" s="15"/>
@@ -1479,10 +1511,13 @@
       <c r="J29" t="b">
         <v>1</v>
       </c>
+      <c r="K29" t="b">
+        <v>1</v>
+      </c>
       <c r="P29" s="9"/>
       <c r="Q29" s="11">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="R29" s="14"/>
       <c r="S29" s="15"/>
@@ -1540,10 +1575,13 @@
       <c r="J31" t="b">
         <v>1</v>
       </c>
+      <c r="K31" t="b">
+        <v>1</v>
+      </c>
       <c r="P31" s="9"/>
       <c r="Q31" s="11">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="R31" s="14"/>
       <c r="S31" s="15"/>
@@ -1635,10 +1673,13 @@
       <c r="J35" t="b">
         <v>1</v>
       </c>
+      <c r="K35" t="b">
+        <v>1</v>
+      </c>
       <c r="P35" s="9"/>
       <c r="Q35" s="11">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="R35" s="14"/>
       <c r="S35" s="15"/>
@@ -1671,10 +1712,13 @@
       <c r="J36" t="b">
         <v>1</v>
       </c>
+      <c r="K36" t="b">
+        <v>1</v>
+      </c>
       <c r="P36" s="9"/>
       <c r="Q36" s="11">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="R36" s="14"/>
       <c r="S36" s="15"/>
@@ -1689,10 +1733,13 @@
       <c r="G37" t="b">
         <v>1</v>
       </c>
+      <c r="K37" t="b">
+        <v>1</v>
+      </c>
       <c r="P37" s="9"/>
       <c r="Q37" s="11">
-        <f>C37+D37+E37+F37+G37+H37+I37+J37+K37+L37+M37+N37+O37+P37</f>
-        <v>2</v>
+        <f t="shared" ref="Q37:Q46" si="1">C37+D37+E37+F37+G37+H37+I37+J37+K37+L37+M37+N37+O37+P37</f>
+        <v>3</v>
       </c>
       <c r="R37" s="14"/>
       <c r="S37" s="15"/>
@@ -1719,7 +1766,7 @@
       </c>
       <c r="P38" s="9"/>
       <c r="Q38" s="11">
-        <f>C38+D38+E38+F38+G38+H38+I38+J38+K38+L38+M38+N38+O38+P38</f>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="R38" s="14"/>
@@ -1752,7 +1799,7 @@
       </c>
       <c r="P39" s="9"/>
       <c r="Q39" s="11">
-        <f>C39+D39+E39+F39+G39+H39+I39+J39+K39+L39+M39+N39+O39+P39</f>
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
       <c r="R39" s="14"/>
@@ -1768,7 +1815,7 @@
       </c>
       <c r="P40" s="9"/>
       <c r="Q40" s="11">
-        <f>C40+D40+E40+F40+G40+H40+I40+J40+K40+L40+M40+N40+O40+P40</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="R40" s="14"/>
@@ -1796,7 +1843,7 @@
       </c>
       <c r="P41" s="9"/>
       <c r="Q41" s="11">
-        <f>C41+D41+E41+F41+G41+H41+I41+J41+K41+L41+M41+N41+O41+P41</f>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="R41" s="14"/>
@@ -1807,23 +1854,12 @@
         <v>61</v>
       </c>
       <c r="C42" s="5"/>
-      <c r="D42" s="20"/>
-      <c r="E42" s="20"/>
-      <c r="F42" s="20"/>
-      <c r="G42" s="20"/>
-      <c r="H42" s="20"/>
-      <c r="I42" s="20"/>
-      <c r="J42" s="20" t="b">
-        <v>1</v>
-      </c>
-      <c r="K42" s="20"/>
-      <c r="L42" s="20"/>
-      <c r="M42" s="20"/>
-      <c r="N42" s="20"/>
-      <c r="O42" s="20"/>
+      <c r="J42" t="b">
+        <v>1</v>
+      </c>
       <c r="P42" s="9"/>
       <c r="Q42" s="11">
-        <f>C42+D42+E42+F42+G42+H42+I42+J42+K42+L42+M42+N42+O42+P42</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="R42" s="14"/>
@@ -1848,7 +1884,7 @@
       </c>
       <c r="P43" s="9"/>
       <c r="Q43" s="11">
-        <f>C43+D43+E43+F43+G43+H43+I43+J43+K43+L43+M43+N43+O43+P43</f>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="R43" s="14"/>
@@ -1879,7 +1915,7 @@
       </c>
       <c r="P44" s="9"/>
       <c r="Q44" s="11">
-        <f>C44+D44+E44+F44+G44+H44+I44+J44+K44+L44+M44+N44+O44+P44</f>
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
       <c r="R44" s="14"/>
@@ -1899,10 +1935,13 @@
       <c r="I45" t="b">
         <v>1</v>
       </c>
+      <c r="K45" t="b">
+        <v>1</v>
+      </c>
       <c r="P45" s="9"/>
       <c r="Q45" s="11">
-        <f>C45+D45+E45+F45+G45+H45+I45+J45+K45+L45+M45+N45+O45+P45</f>
-        <v>3</v>
+        <f t="shared" si="1"/>
+        <v>4</v>
       </c>
       <c r="R45" s="14"/>
       <c r="S45" s="15"/>
@@ -1938,17 +1977,44 @@
       <c r="O46" s="7"/>
       <c r="P46" s="10"/>
       <c r="Q46" s="11">
-        <f>C46+D46+E46+F46+G46+H46+I46+J46+K46+L46+M46+N46+O46+P46</f>
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
       <c r="R46" s="16"/>
       <c r="S46" s="17"/>
+    </row>
+    <row r="47" spans="2:19">
+      <c r="B47" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="C47" s="6"/>
+      <c r="D47" s="7"/>
+      <c r="E47" s="7"/>
+      <c r="F47" s="7"/>
+      <c r="G47" s="7"/>
+      <c r="H47" s="7"/>
+      <c r="I47" s="7"/>
+      <c r="J47" s="7"/>
+      <c r="K47" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="L47" s="7"/>
+      <c r="M47" s="7"/>
+      <c r="N47" s="7"/>
+      <c r="O47" s="7"/>
+      <c r="P47" s="10"/>
+      <c r="Q47" s="11">
+        <f t="shared" ref="Q47" si="2">C47+D47+E47+F47+G47+H47+I47+J47+K47+L47+M47+N47+O47+P47</f>
+        <v>1</v>
+      </c>
+      <c r="R47" s="16"/>
+      <c r="S47" s="17"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B37:S46">
     <sortCondition ref="B46"/>
   </sortState>
-  <conditionalFormatting sqref="Q3:Q46">
+  <conditionalFormatting sqref="Q3:Q47">
     <cfRule type="cellIs" dxfId="0" priority="2" operator="lessThan">
       <formula>4</formula>
     </cfRule>

</xml_diff>

<commit_message>
Laborator 05.12.2023 - Login part 1
</commit_message>
<xml_diff>
--- a/MetodeAvansate/Prezenta.xlsx
+++ b/MetodeAvansate/Prezenta.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\remus\Documents\GitHub\Facultate_2023\MetodeAvansate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13B8DB4F-96FE-4BD6-B8E2-8C49A9C20BB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{669517FD-44AC-4673-98BE-5CA82936635C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -417,7 +417,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -433,9 +432,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -444,6 +440,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -730,8 +732,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:S47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="J53" sqref="J53"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
@@ -798,7 +800,7 @@
       </c>
     </row>
     <row r="3" spans="2:19">
-      <c r="B3" s="18" t="s">
+      <c r="B3" s="16" t="s">
         <v>43</v>
       </c>
       <c r="C3" s="3"/>
@@ -823,15 +825,15 @@
       <c r="N3" s="4"/>
       <c r="O3" s="4"/>
       <c r="P3" s="8"/>
-      <c r="Q3" s="11">
-        <f t="shared" ref="Q3:Q36" si="0">C3+D3+E3+F3+G3+H3+I3+J3+K3+L3+M3+N3+O3+P3</f>
+      <c r="Q3" s="10">
+        <f t="shared" ref="Q3:Q47" si="0">C3+D3+E3+F3+G3+H3+I3+J3+K3+L3+M3+N3+O3+P3</f>
         <v>4</v>
       </c>
-      <c r="R3" s="12"/>
-      <c r="S3" s="13"/>
+      <c r="R3" s="11"/>
+      <c r="S3" s="12"/>
     </row>
     <row r="4" spans="2:19">
-      <c r="B4" s="18" t="s">
+      <c r="B4" s="16" t="s">
         <v>46</v>
       </c>
       <c r="C4" s="5"/>
@@ -839,15 +841,15 @@
         <v>1</v>
       </c>
       <c r="P4" s="9"/>
-      <c r="Q4" s="11">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="R4" s="14"/>
-      <c r="S4" s="15"/>
+      <c r="Q4" s="10">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="R4" s="13"/>
+      <c r="S4" s="14"/>
     </row>
     <row r="5" spans="2:19">
-      <c r="B5" s="18" t="s">
+      <c r="B5" s="16" t="s">
         <v>50</v>
       </c>
       <c r="C5" s="5"/>
@@ -855,15 +857,15 @@
         <v>1</v>
       </c>
       <c r="P5" s="9"/>
-      <c r="Q5" s="11">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="R5" s="14"/>
-      <c r="S5" s="15"/>
+      <c r="Q5" s="10">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="R5" s="13"/>
+      <c r="S5" s="14"/>
     </row>
     <row r="6" spans="2:19">
-      <c r="B6" s="18" t="s">
+      <c r="B6" s="16" t="s">
         <v>38</v>
       </c>
       <c r="C6" s="5"/>
@@ -891,16 +893,19 @@
       <c r="K6" t="b">
         <v>1</v>
       </c>
+      <c r="L6" t="b">
+        <v>1</v>
+      </c>
       <c r="P6" s="9"/>
-      <c r="Q6" s="11">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="R6" s="14"/>
-      <c r="S6" s="15"/>
+      <c r="Q6" s="10">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="R6" s="13"/>
+      <c r="S6" s="14"/>
     </row>
     <row r="7" spans="2:19">
-      <c r="B7" s="18" t="s">
+      <c r="B7" s="16" t="s">
         <v>56</v>
       </c>
       <c r="C7" s="5"/>
@@ -920,15 +925,15 @@
         <v>1</v>
       </c>
       <c r="P7" s="9"/>
-      <c r="Q7" s="11">
+      <c r="Q7" s="10">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="R7" s="14"/>
-      <c r="S7" s="15"/>
+      <c r="R7" s="13"/>
+      <c r="S7" s="14"/>
     </row>
     <row r="8" spans="2:19">
-      <c r="B8" s="18" t="s">
+      <c r="B8" s="16" t="s">
         <v>47</v>
       </c>
       <c r="C8" s="5"/>
@@ -945,15 +950,15 @@
         <v>1</v>
       </c>
       <c r="P8" s="9"/>
-      <c r="Q8" s="11">
+      <c r="Q8" s="10">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="R8" s="14"/>
-      <c r="S8" s="15"/>
+      <c r="R8" s="13"/>
+      <c r="S8" s="14"/>
     </row>
     <row r="9" spans="2:19">
-      <c r="B9" s="18" t="s">
+      <c r="B9" s="16" t="s">
         <v>57</v>
       </c>
       <c r="C9" s="5"/>
@@ -964,15 +969,15 @@
         <v>1</v>
       </c>
       <c r="P9" s="9"/>
-      <c r="Q9" s="11">
+      <c r="Q9" s="10">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="R9" s="14"/>
-      <c r="S9" s="15"/>
+      <c r="R9" s="13"/>
+      <c r="S9" s="14"/>
     </row>
     <row r="10" spans="2:19">
-      <c r="B10" s="18" t="s">
+      <c r="B10" s="16" t="s">
         <v>39</v>
       </c>
       <c r="C10" s="5"/>
@@ -1000,16 +1005,19 @@
       <c r="K10" t="b">
         <v>1</v>
       </c>
+      <c r="L10" t="b">
+        <v>1</v>
+      </c>
       <c r="P10" s="9"/>
-      <c r="Q10" s="11">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="R10" s="14"/>
-      <c r="S10" s="15"/>
+      <c r="Q10" s="10">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="R10" s="13"/>
+      <c r="S10" s="14"/>
     </row>
     <row r="11" spans="2:19">
-      <c r="B11" s="18" t="s">
+      <c r="B11" s="16" t="s">
         <v>59</v>
       </c>
       <c r="C11" s="5"/>
@@ -1020,15 +1028,15 @@
         <v>1</v>
       </c>
       <c r="P11" s="9"/>
-      <c r="Q11" s="11">
+      <c r="Q11" s="10">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="R11" s="14"/>
-      <c r="S11" s="15"/>
+      <c r="R11" s="13"/>
+      <c r="S11" s="14"/>
     </row>
     <row r="12" spans="2:19">
-      <c r="B12" s="18" t="s">
+      <c r="B12" s="16" t="s">
         <v>60</v>
       </c>
       <c r="C12" s="5"/>
@@ -1036,15 +1044,15 @@
         <v>1</v>
       </c>
       <c r="P12" s="9"/>
-      <c r="Q12" s="11">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="R12" s="14"/>
-      <c r="S12" s="15"/>
+      <c r="Q12" s="10">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="R12" s="13"/>
+      <c r="S12" s="14"/>
     </row>
     <row r="13" spans="2:19">
-      <c r="B13" s="18" t="s">
+      <c r="B13" s="16" t="s">
         <v>32</v>
       </c>
       <c r="C13" s="5" t="b">
@@ -1054,30 +1062,30 @@
         <v>1</v>
       </c>
       <c r="P13" s="9"/>
-      <c r="Q13" s="11">
+      <c r="Q13" s="10">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="R13" s="14"/>
-      <c r="S13" s="15"/>
+      <c r="R13" s="13"/>
+      <c r="S13" s="14"/>
     </row>
     <row r="14" spans="2:19">
-      <c r="B14" s="18" t="s">
+      <c r="B14" s="16" t="s">
         <v>28</v>
       </c>
       <c r="C14" s="5" t="b">
         <v>1</v>
       </c>
       <c r="P14" s="9"/>
-      <c r="Q14" s="11">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="R14" s="14"/>
-      <c r="S14" s="15"/>
+      <c r="Q14" s="10">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="R14" s="13"/>
+      <c r="S14" s="14"/>
     </row>
     <row r="15" spans="2:19">
-      <c r="B15" s="18" t="s">
+      <c r="B15" s="16" t="s">
         <v>27</v>
       </c>
       <c r="C15" s="5" t="b">
@@ -1102,15 +1110,15 @@
         <v>1</v>
       </c>
       <c r="P15" s="9"/>
-      <c r="Q15" s="11">
+      <c r="Q15" s="10">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="R15" s="14"/>
-      <c r="S15" s="15"/>
+      <c r="R15" s="13"/>
+      <c r="S15" s="14"/>
     </row>
     <row r="16" spans="2:19">
-      <c r="B16" s="18" t="s">
+      <c r="B16" s="16" t="s">
         <v>29</v>
       </c>
       <c r="C16" s="5" t="b">
@@ -1135,15 +1143,15 @@
         <v>1</v>
       </c>
       <c r="P16" s="9"/>
-      <c r="Q16" s="11">
+      <c r="Q16" s="10">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="R16" s="14"/>
-      <c r="S16" s="15"/>
+      <c r="R16" s="13"/>
+      <c r="S16" s="14"/>
     </row>
     <row r="17" spans="2:19">
-      <c r="B17" s="18" t="s">
+      <c r="B17" s="16" t="s">
         <v>33</v>
       </c>
       <c r="C17" s="5" t="b">
@@ -1173,16 +1181,19 @@
       <c r="K17" t="b">
         <v>1</v>
       </c>
+      <c r="L17" t="b">
+        <v>1</v>
+      </c>
       <c r="P17" s="9"/>
-      <c r="Q17" s="11">
-        <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
-      <c r="R17" s="14"/>
-      <c r="S17" s="15"/>
+      <c r="Q17" s="10">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="R17" s="13"/>
+      <c r="S17" s="14"/>
     </row>
     <row r="18" spans="2:19">
-      <c r="B18" s="18" t="s">
+      <c r="B18" s="16" t="s">
         <v>31</v>
       </c>
       <c r="C18" s="5" t="b">
@@ -1212,16 +1223,19 @@
       <c r="K18" t="b">
         <v>1</v>
       </c>
+      <c r="L18" t="b">
+        <v>1</v>
+      </c>
       <c r="P18" s="9"/>
-      <c r="Q18" s="11">
-        <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
-      <c r="R18" s="14"/>
-      <c r="S18" s="15"/>
+      <c r="Q18" s="10">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="R18" s="13"/>
+      <c r="S18" s="14"/>
     </row>
     <row r="19" spans="2:19">
-      <c r="B19" s="18" t="s">
+      <c r="B19" s="16" t="s">
         <v>18</v>
       </c>
       <c r="C19" s="5" t="b">
@@ -1246,15 +1260,15 @@
         <v>1</v>
       </c>
       <c r="P19" s="9"/>
-      <c r="Q19" s="11">
+      <c r="Q19" s="10">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="R19" s="14"/>
-      <c r="S19" s="15"/>
+      <c r="R19" s="13"/>
+      <c r="S19" s="14"/>
     </row>
     <row r="20" spans="2:19">
-      <c r="B20" s="18" t="s">
+      <c r="B20" s="16" t="s">
         <v>54</v>
       </c>
       <c r="C20" s="5"/>
@@ -1265,15 +1279,15 @@
         <v>1</v>
       </c>
       <c r="P20" s="9"/>
-      <c r="Q20" s="11">
+      <c r="Q20" s="10">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="R20" s="14"/>
-      <c r="S20" s="15"/>
+      <c r="R20" s="13"/>
+      <c r="S20" s="14"/>
     </row>
     <row r="21" spans="2:19">
-      <c r="B21" s="18" t="s">
+      <c r="B21" s="16" t="s">
         <v>30</v>
       </c>
       <c r="C21" s="5" t="b">
@@ -1300,16 +1314,19 @@
       <c r="K21" t="b">
         <v>1</v>
       </c>
+      <c r="L21" t="b">
+        <v>1</v>
+      </c>
       <c r="P21" s="9"/>
-      <c r="Q21" s="11">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="R21" s="14"/>
-      <c r="S21" s="15"/>
+      <c r="Q21" s="10">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="R21" s="13"/>
+      <c r="S21" s="14"/>
     </row>
     <row r="22" spans="2:19">
-      <c r="B22" s="18" t="s">
+      <c r="B22" s="16" t="s">
         <v>51</v>
       </c>
       <c r="C22" s="5"/>
@@ -1325,16 +1342,19 @@
       <c r="I22" t="b">
         <v>1</v>
       </c>
+      <c r="L22" t="b">
+        <v>1</v>
+      </c>
       <c r="P22" s="9"/>
-      <c r="Q22" s="11">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="R22" s="14"/>
-      <c r="S22" s="15"/>
+      <c r="Q22" s="10">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="R22" s="13"/>
+      <c r="S22" s="14"/>
     </row>
     <row r="23" spans="2:19">
-      <c r="B23" s="18" t="s">
+      <c r="B23" s="16" t="s">
         <v>34</v>
       </c>
       <c r="C23" s="5" t="b">
@@ -1356,15 +1376,15 @@
         <v>1</v>
       </c>
       <c r="P23" s="9"/>
-      <c r="Q23" s="11">
+      <c r="Q23" s="10">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="R23" s="14"/>
-      <c r="S23" s="15"/>
+      <c r="R23" s="13"/>
+      <c r="S23" s="14"/>
     </row>
     <row r="24" spans="2:19">
-      <c r="B24" s="18" t="s">
+      <c r="B24" s="16" t="s">
         <v>41</v>
       </c>
       <c r="C24" s="5"/>
@@ -1372,15 +1392,15 @@
         <v>1</v>
       </c>
       <c r="P24" s="9"/>
-      <c r="Q24" s="11">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="R24" s="14"/>
-      <c r="S24" s="15"/>
+      <c r="Q24" s="10">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="R24" s="13"/>
+      <c r="S24" s="14"/>
     </row>
     <row r="25" spans="2:19">
-      <c r="B25" s="18" t="s">
+      <c r="B25" s="16" t="s">
         <v>19</v>
       </c>
       <c r="C25" s="5" t="b">
@@ -1393,30 +1413,30 @@
         <v>1</v>
       </c>
       <c r="P25" s="9"/>
-      <c r="Q25" s="11">
+      <c r="Q25" s="10">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="R25" s="14"/>
-      <c r="S25" s="15"/>
+      <c r="R25" s="13"/>
+      <c r="S25" s="14"/>
     </row>
     <row r="26" spans="2:19">
-      <c r="B26" s="18" t="s">
+      <c r="B26" s="16" t="s">
         <v>20</v>
       </c>
       <c r="C26" s="5" t="b">
         <v>1</v>
       </c>
       <c r="P26" s="9"/>
-      <c r="Q26" s="11">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="R26" s="14"/>
-      <c r="S26" s="15"/>
+      <c r="Q26" s="10">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="R26" s="13"/>
+      <c r="S26" s="14"/>
     </row>
     <row r="27" spans="2:19">
-      <c r="B27" s="18" t="s">
+      <c r="B27" s="16" t="s">
         <v>37</v>
       </c>
       <c r="C27" s="5"/>
@@ -1442,15 +1462,15 @@
         <v>1</v>
       </c>
       <c r="P27" s="9"/>
-      <c r="Q27" s="11">
+      <c r="Q27" s="10">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="R27" s="14"/>
-      <c r="S27" s="15"/>
+      <c r="R27" s="13"/>
+      <c r="S27" s="14"/>
     </row>
     <row r="28" spans="2:19">
-      <c r="B28" s="18" t="s">
+      <c r="B28" s="16" t="s">
         <v>21</v>
       </c>
       <c r="C28" s="5" t="b">
@@ -1480,16 +1500,19 @@
       <c r="K28" t="b">
         <v>1</v>
       </c>
+      <c r="L28" t="b">
+        <v>1</v>
+      </c>
       <c r="P28" s="9"/>
-      <c r="Q28" s="11">
-        <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
-      <c r="R28" s="14"/>
-      <c r="S28" s="15"/>
+      <c r="Q28" s="10">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="R28" s="13"/>
+      <c r="S28" s="14"/>
     </row>
     <row r="29" spans="2:19">
-      <c r="B29" s="18" t="s">
+      <c r="B29" s="16" t="s">
         <v>45</v>
       </c>
       <c r="C29" s="5"/>
@@ -1515,15 +1538,15 @@
         <v>1</v>
       </c>
       <c r="P29" s="9"/>
-      <c r="Q29" s="11">
+      <c r="Q29" s="10">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="R29" s="14"/>
-      <c r="S29" s="15"/>
+      <c r="R29" s="13"/>
+      <c r="S29" s="14"/>
     </row>
     <row r="30" spans="2:19">
-      <c r="B30" s="18" t="s">
+      <c r="B30" s="16" t="s">
         <v>22</v>
       </c>
       <c r="C30" s="5" t="b">
@@ -1550,16 +1573,19 @@
       <c r="J30" t="b">
         <v>1</v>
       </c>
+      <c r="K30" t="b">
+        <v>1</v>
+      </c>
       <c r="P30" s="9"/>
-      <c r="Q30" s="11">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="R30" s="14"/>
-      <c r="S30" s="15"/>
+      <c r="Q30" s="10">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="R30" s="13"/>
+      <c r="S30" s="14"/>
     </row>
     <row r="31" spans="2:19">
-      <c r="B31" s="18" t="s">
+      <c r="B31" s="16" t="s">
         <v>44</v>
       </c>
       <c r="C31" s="5"/>
@@ -1579,15 +1605,15 @@
         <v>1</v>
       </c>
       <c r="P31" s="9"/>
-      <c r="Q31" s="11">
+      <c r="Q31" s="10">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="R31" s="14"/>
-      <c r="S31" s="15"/>
+      <c r="R31" s="13"/>
+      <c r="S31" s="14"/>
     </row>
     <row r="32" spans="2:19">
-      <c r="B32" s="18" t="s">
+      <c r="B32" s="16" t="s">
         <v>36</v>
       </c>
       <c r="C32" s="5"/>
@@ -1595,424 +1621,425 @@
         <v>1</v>
       </c>
       <c r="P32" s="9"/>
-      <c r="Q32" s="11">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="R32" s="14"/>
-      <c r="S32" s="15"/>
+      <c r="Q32" s="10">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="R32" s="13"/>
+      <c r="S32" s="14"/>
     </row>
     <row r="33" spans="2:19">
-      <c r="B33" s="18" t="s">
+      <c r="B33" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="C33" s="5"/>
+      <c r="K33" t="b">
+        <v>1</v>
+      </c>
+      <c r="P33" s="9"/>
+      <c r="Q33" s="10">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="R33" s="13"/>
+      <c r="S33" s="14"/>
+    </row>
+    <row r="34" spans="2:19">
+      <c r="B34" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="C33" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="E33" t="b">
-        <v>1</v>
-      </c>
-      <c r="F33" t="b">
-        <v>1</v>
-      </c>
-      <c r="I33" t="b">
-        <v>1</v>
-      </c>
-      <c r="P33" s="9"/>
-      <c r="Q33" s="11">
+      <c r="C34" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="E34" t="b">
+        <v>1</v>
+      </c>
+      <c r="F34" t="b">
+        <v>1</v>
+      </c>
+      <c r="I34" t="b">
+        <v>1</v>
+      </c>
+      <c r="P34" s="9"/>
+      <c r="Q34" s="10">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="R33" s="14"/>
-      <c r="S33" s="15"/>
-    </row>
-    <row r="34" spans="2:19">
-      <c r="B34" s="18" t="s">
+      <c r="R34" s="13"/>
+      <c r="S34" s="14"/>
+    </row>
+    <row r="35" spans="2:19">
+      <c r="B35" s="16" t="s">
         <v>58</v>
       </c>
-      <c r="C34" s="5"/>
-      <c r="H34" t="b">
-        <v>1</v>
-      </c>
-      <c r="I34" t="b">
-        <v>1</v>
-      </c>
-      <c r="P34" s="9"/>
-      <c r="Q34" s="11">
+      <c r="C35" s="5"/>
+      <c r="H35" t="b">
+        <v>1</v>
+      </c>
+      <c r="I35" t="b">
+        <v>1</v>
+      </c>
+      <c r="P35" s="9"/>
+      <c r="Q35" s="10">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="R34" s="14"/>
-      <c r="S34" s="15"/>
-    </row>
-    <row r="35" spans="2:19">
-      <c r="B35" s="18" t="s">
+      <c r="R35" s="13"/>
+      <c r="S35" s="14"/>
+    </row>
+    <row r="36" spans="2:19">
+      <c r="B36" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="C35" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="D35" t="b">
-        <v>1</v>
-      </c>
-      <c r="E35" t="b">
-        <v>1</v>
-      </c>
-      <c r="F35" t="b">
-        <v>1</v>
-      </c>
-      <c r="G35" t="b">
-        <v>1</v>
-      </c>
-      <c r="H35" t="b">
-        <v>1</v>
-      </c>
-      <c r="I35" t="b">
-        <v>1</v>
-      </c>
-      <c r="J35" t="b">
-        <v>1</v>
-      </c>
-      <c r="K35" t="b">
-        <v>1</v>
-      </c>
-      <c r="P35" s="9"/>
-      <c r="Q35" s="11">
-        <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
-      <c r="R35" s="14"/>
-      <c r="S35" s="15"/>
-    </row>
-    <row r="36" spans="2:19">
-      <c r="B36" s="18" t="s">
+      <c r="C36" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="D36" t="b">
+        <v>1</v>
+      </c>
+      <c r="E36" t="b">
+        <v>1</v>
+      </c>
+      <c r="F36" t="b">
+        <v>1</v>
+      </c>
+      <c r="G36" t="b">
+        <v>1</v>
+      </c>
+      <c r="H36" t="b">
+        <v>1</v>
+      </c>
+      <c r="I36" t="b">
+        <v>1</v>
+      </c>
+      <c r="J36" t="b">
+        <v>1</v>
+      </c>
+      <c r="K36" t="b">
+        <v>1</v>
+      </c>
+      <c r="L36" t="b">
+        <v>1</v>
+      </c>
+      <c r="P36" s="9"/>
+      <c r="Q36" s="10">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="R36" s="13"/>
+      <c r="S36" s="14"/>
+    </row>
+    <row r="37" spans="2:19">
+      <c r="B37" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="C36" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="D36" t="b">
-        <v>1</v>
-      </c>
-      <c r="E36" t="b">
-        <v>1</v>
-      </c>
-      <c r="F36" t="b">
-        <v>1</v>
-      </c>
-      <c r="G36" t="b">
-        <v>1</v>
-      </c>
-      <c r="H36" t="b">
-        <v>1</v>
-      </c>
-      <c r="I36" t="b">
-        <v>1</v>
-      </c>
-      <c r="J36" t="b">
-        <v>1</v>
-      </c>
-      <c r="K36" t="b">
-        <v>1</v>
-      </c>
-      <c r="P36" s="9"/>
-      <c r="Q36" s="11">
-        <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
-      <c r="R36" s="14"/>
-      <c r="S36" s="15"/>
-    </row>
-    <row r="37" spans="2:19">
-      <c r="B37" s="18" t="s">
+      <c r="C37" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="D37" t="b">
+        <v>1</v>
+      </c>
+      <c r="E37" t="b">
+        <v>1</v>
+      </c>
+      <c r="F37" t="b">
+        <v>1</v>
+      </c>
+      <c r="G37" t="b">
+        <v>1</v>
+      </c>
+      <c r="H37" t="b">
+        <v>1</v>
+      </c>
+      <c r="I37" t="b">
+        <v>1</v>
+      </c>
+      <c r="J37" t="b">
+        <v>1</v>
+      </c>
+      <c r="K37" t="b">
+        <v>1</v>
+      </c>
+      <c r="L37" t="b">
+        <v>1</v>
+      </c>
+      <c r="P37" s="9"/>
+      <c r="Q37" s="10">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="R37" s="13"/>
+      <c r="S37" s="14"/>
+    </row>
+    <row r="38" spans="2:19">
+      <c r="B38" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="C37" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="G37" t="b">
-        <v>1</v>
-      </c>
-      <c r="K37" t="b">
-        <v>1</v>
-      </c>
-      <c r="P37" s="9"/>
-      <c r="Q37" s="11">
-        <f t="shared" ref="Q37:Q46" si="1">C37+D37+E37+F37+G37+H37+I37+J37+K37+L37+M37+N37+O37+P37</f>
+      <c r="C38" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="G38" t="b">
+        <v>1</v>
+      </c>
+      <c r="K38" t="b">
+        <v>1</v>
+      </c>
+      <c r="P38" s="9"/>
+      <c r="Q38" s="10">
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="R37" s="14"/>
-      <c r="S37" s="15"/>
-    </row>
-    <row r="38" spans="2:19">
-      <c r="B38" s="18" t="s">
+      <c r="R38" s="13"/>
+      <c r="S38" s="14"/>
+    </row>
+    <row r="39" spans="2:19">
+      <c r="B39" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="C38" s="5"/>
-      <c r="E38" t="b">
-        <v>1</v>
-      </c>
-      <c r="F38" t="b">
-        <v>1</v>
-      </c>
-      <c r="G38" t="b">
-        <v>1</v>
-      </c>
-      <c r="I38" t="b">
-        <v>1</v>
-      </c>
-      <c r="J38" t="b">
-        <v>1</v>
-      </c>
-      <c r="P38" s="9"/>
-      <c r="Q38" s="11">
-        <f t="shared" si="1"/>
+      <c r="C39" s="5"/>
+      <c r="E39" t="b">
+        <v>1</v>
+      </c>
+      <c r="F39" t="b">
+        <v>1</v>
+      </c>
+      <c r="G39" t="b">
+        <v>1</v>
+      </c>
+      <c r="I39" t="b">
+        <v>1</v>
+      </c>
+      <c r="J39" t="b">
+        <v>1</v>
+      </c>
+      <c r="P39" s="9"/>
+      <c r="Q39" s="10">
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="R38" s="14"/>
-      <c r="S38" s="15"/>
-    </row>
-    <row r="39" spans="2:19">
-      <c r="B39" s="18" t="s">
+      <c r="R39" s="13"/>
+      <c r="S39" s="14"/>
+    </row>
+    <row r="40" spans="2:19">
+      <c r="B40" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="C39" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="D39" t="b">
-        <v>1</v>
-      </c>
-      <c r="E39" t="b">
-        <v>1</v>
-      </c>
-      <c r="F39" t="b">
-        <v>1</v>
-      </c>
-      <c r="G39" t="b">
-        <v>1</v>
-      </c>
-      <c r="I39" t="b">
-        <v>1</v>
-      </c>
-      <c r="J39" t="b">
-        <v>1</v>
-      </c>
-      <c r="P39" s="9"/>
-      <c r="Q39" s="11">
-        <f t="shared" si="1"/>
+      <c r="C40" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="D40" t="b">
+        <v>1</v>
+      </c>
+      <c r="E40" t="b">
+        <v>1</v>
+      </c>
+      <c r="F40" t="b">
+        <v>1</v>
+      </c>
+      <c r="G40" t="b">
+        <v>1</v>
+      </c>
+      <c r="I40" t="b">
+        <v>1</v>
+      </c>
+      <c r="J40" t="b">
+        <v>1</v>
+      </c>
+      <c r="P40" s="9"/>
+      <c r="Q40" s="10">
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="R39" s="14"/>
-      <c r="S39" s="15"/>
-    </row>
-    <row r="40" spans="2:19">
-      <c r="B40" s="18" t="s">
+      <c r="R40" s="13"/>
+      <c r="S40" s="14"/>
+    </row>
+    <row r="41" spans="2:19">
+      <c r="B41" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="C40" s="5"/>
-      <c r="E40" t="b">
-        <v>1</v>
-      </c>
-      <c r="P40" s="9"/>
-      <c r="Q40" s="11">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="R40" s="14"/>
-      <c r="S40" s="15"/>
-    </row>
-    <row r="41" spans="2:19">
-      <c r="B41" s="18" t="s">
+      <c r="C41" s="5"/>
+      <c r="E41" t="b">
+        <v>1</v>
+      </c>
+      <c r="P41" s="9"/>
+      <c r="Q41" s="10">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="R41" s="13"/>
+      <c r="S41" s="14"/>
+    </row>
+    <row r="42" spans="2:19">
+      <c r="B42" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="C41" s="5"/>
-      <c r="D41" t="b">
-        <v>1</v>
-      </c>
-      <c r="E41" t="b">
-        <v>1</v>
-      </c>
-      <c r="G41" t="b">
-        <v>1</v>
-      </c>
-      <c r="H41" t="b">
-        <v>1</v>
-      </c>
-      <c r="I41" t="b">
-        <v>1</v>
-      </c>
-      <c r="P41" s="9"/>
-      <c r="Q41" s="11">
-        <f t="shared" si="1"/>
+      <c r="C42" s="5"/>
+      <c r="D42" t="b">
+        <v>1</v>
+      </c>
+      <c r="E42" t="b">
+        <v>1</v>
+      </c>
+      <c r="G42" t="b">
+        <v>1</v>
+      </c>
+      <c r="H42" t="b">
+        <v>1</v>
+      </c>
+      <c r="I42" t="b">
+        <v>1</v>
+      </c>
+      <c r="L42" t="b">
+        <v>1</v>
+      </c>
+      <c r="P42" s="9"/>
+      <c r="Q42" s="10">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="R42" s="13"/>
+      <c r="S42" s="14"/>
+    </row>
+    <row r="43" spans="2:19">
+      <c r="B43" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="C43" s="5"/>
+      <c r="J43" t="b">
+        <v>1</v>
+      </c>
+      <c r="P43" s="9"/>
+      <c r="Q43" s="10">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="R43" s="13"/>
+      <c r="S43" s="14"/>
+    </row>
+    <row r="44" spans="2:19">
+      <c r="B44" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="C44" s="5"/>
+      <c r="G44" t="b">
+        <v>1</v>
+      </c>
+      <c r="H44" t="b">
+        <v>1</v>
+      </c>
+      <c r="I44" t="b">
+        <v>1</v>
+      </c>
+      <c r="J44" t="b">
+        <v>1</v>
+      </c>
+      <c r="P44" s="9"/>
+      <c r="Q44" s="10">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="R44" s="13"/>
+      <c r="S44" s="14"/>
+    </row>
+    <row r="45" spans="2:19">
+      <c r="B45" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="C45" s="5"/>
+      <c r="D45" t="b">
+        <v>1</v>
+      </c>
+      <c r="E45" t="b">
+        <v>1</v>
+      </c>
+      <c r="F45" t="b">
+        <v>1</v>
+      </c>
+      <c r="G45" t="b">
+        <v>1</v>
+      </c>
+      <c r="H45" t="b">
+        <v>1</v>
+      </c>
+      <c r="I45" t="b">
+        <v>1</v>
+      </c>
+      <c r="P45" s="9"/>
+      <c r="Q45" s="10">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="R45" s="13"/>
+      <c r="S45" s="14"/>
+    </row>
+    <row r="46" spans="2:19">
+      <c r="B46" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="C46" s="5"/>
+      <c r="F46" t="b">
+        <v>1</v>
+      </c>
+      <c r="G46" t="b">
+        <v>1</v>
+      </c>
+      <c r="I46" t="b">
+        <v>1</v>
+      </c>
+      <c r="K46" t="b">
+        <v>1</v>
+      </c>
+      <c r="L46" t="b">
+        <v>1</v>
+      </c>
+      <c r="P46" s="9"/>
+      <c r="Q46" s="10">
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="R41" s="14"/>
-      <c r="S41" s="15"/>
-    </row>
-    <row r="42" spans="2:19">
-      <c r="B42" s="18" t="s">
-        <v>61</v>
-      </c>
-      <c r="C42" s="5"/>
-      <c r="J42" t="b">
-        <v>1</v>
-      </c>
-      <c r="P42" s="9"/>
-      <c r="Q42" s="11">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="R42" s="14"/>
-      <c r="S42" s="15"/>
-    </row>
-    <row r="43" spans="2:19">
-      <c r="B43" s="18" t="s">
-        <v>55</v>
-      </c>
-      <c r="C43" s="5"/>
-      <c r="G43" t="b">
-        <v>1</v>
-      </c>
-      <c r="H43" t="b">
-        <v>1</v>
-      </c>
-      <c r="I43" t="b">
-        <v>1</v>
-      </c>
-      <c r="J43" t="b">
-        <v>1</v>
-      </c>
-      <c r="P43" s="9"/>
-      <c r="Q43" s="11">
-        <f t="shared" si="1"/>
-        <v>4</v>
-      </c>
-      <c r="R43" s="14"/>
-      <c r="S43" s="15"/>
-    </row>
-    <row r="44" spans="2:19">
-      <c r="B44" s="19" t="s">
-        <v>42</v>
-      </c>
-      <c r="C44" s="5"/>
-      <c r="D44" t="b">
-        <v>1</v>
-      </c>
-      <c r="E44" t="b">
-        <v>1</v>
-      </c>
-      <c r="F44" t="b">
-        <v>1</v>
-      </c>
-      <c r="G44" t="b">
-        <v>1</v>
-      </c>
-      <c r="H44" t="b">
-        <v>1</v>
-      </c>
-      <c r="I44" t="b">
-        <v>1</v>
-      </c>
-      <c r="P44" s="9"/>
-      <c r="Q44" s="11">
-        <f t="shared" si="1"/>
-        <v>6</v>
-      </c>
-      <c r="R44" s="14"/>
-      <c r="S44" s="15"/>
-    </row>
-    <row r="45" spans="2:19">
-      <c r="B45" s="18" t="s">
-        <v>53</v>
-      </c>
-      <c r="C45" s="5"/>
-      <c r="F45" t="b">
-        <v>1</v>
-      </c>
-      <c r="G45" t="b">
-        <v>1</v>
-      </c>
-      <c r="I45" t="b">
-        <v>1</v>
-      </c>
-      <c r="K45" t="b">
-        <v>1</v>
-      </c>
-      <c r="P45" s="9"/>
-      <c r="Q45" s="11">
-        <f t="shared" si="1"/>
-        <v>4</v>
-      </c>
-      <c r="R45" s="14"/>
-      <c r="S45" s="15"/>
-    </row>
-    <row r="46" spans="2:19">
-      <c r="B46" s="18" t="s">
+      <c r="R46" s="13"/>
+      <c r="S46" s="14"/>
+    </row>
+    <row r="47" spans="2:19">
+      <c r="B47" s="16" t="s">
         <v>49</v>
-      </c>
-      <c r="C46" s="6"/>
-      <c r="D46" s="7"/>
-      <c r="E46" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="F46" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="G46" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="H46" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="I46" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="J46" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="K46" s="7"/>
-      <c r="L46" s="7"/>
-      <c r="M46" s="7"/>
-      <c r="N46" s="7"/>
-      <c r="O46" s="7"/>
-      <c r="P46" s="10"/>
-      <c r="Q46" s="11">
-        <f t="shared" si="1"/>
-        <v>6</v>
-      </c>
-      <c r="R46" s="16"/>
-      <c r="S46" s="17"/>
-    </row>
-    <row r="47" spans="2:19">
-      <c r="B47" s="18" t="s">
-        <v>62</v>
       </c>
       <c r="C47" s="6"/>
       <c r="D47" s="7"/>
-      <c r="E47" s="7"/>
-      <c r="F47" s="7"/>
-      <c r="G47" s="7"/>
-      <c r="H47" s="7"/>
-      <c r="I47" s="7"/>
-      <c r="J47" s="7"/>
-      <c r="K47" s="7" t="b">
-        <v>1</v>
-      </c>
+      <c r="E47" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F47" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="G47" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="H47" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="I47" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="J47" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="K47" s="7"/>
       <c r="L47" s="7"/>
       <c r="M47" s="7"/>
       <c r="N47" s="7"/>
       <c r="O47" s="7"/>
-      <c r="P47" s="10"/>
-      <c r="Q47" s="11">
-        <f t="shared" ref="Q47" si="2">C47+D47+E47+F47+G47+H47+I47+J47+K47+L47+M47+N47+O47+P47</f>
-        <v>1</v>
-      </c>
-      <c r="R47" s="16"/>
-      <c r="S47" s="17"/>
+      <c r="P47" s="7"/>
+      <c r="Q47" s="18">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="R47" s="19"/>
+      <c r="S47" s="15"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B37:S46">
-    <sortCondition ref="B46"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:S47">
+    <sortCondition ref="B47"/>
   </sortState>
   <conditionalFormatting sqref="Q3:Q47">
     <cfRule type="cellIs" dxfId="0" priority="2" operator="lessThan">

</xml_diff>

<commit_message>
laborator 12.12.2023 - Login part 2 + login pe frontend + add article
</commit_message>
<xml_diff>
--- a/MetodeAvansate/Prezenta.xlsx
+++ b/MetodeAvansate/Prezenta.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\remus\Documents\GitHub\Facultate_2023\MetodeAvansate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{669517FD-44AC-4673-98BE-5CA82936635C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4933CF7-AA69-4E3E-A9DC-F201F6C8D9CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -732,8 +732,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:S47"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
@@ -896,10 +896,13 @@
       <c r="L6" t="b">
         <v>1</v>
       </c>
+      <c r="M6" t="b">
+        <v>1</v>
+      </c>
       <c r="P6" s="9"/>
       <c r="Q6" s="10">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="R6" s="13"/>
       <c r="S6" s="14"/>
@@ -1008,10 +1011,13 @@
       <c r="L10" t="b">
         <v>1</v>
       </c>
+      <c r="M10" t="b">
+        <v>1</v>
+      </c>
       <c r="P10" s="9"/>
       <c r="Q10" s="10">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="R10" s="13"/>
       <c r="S10" s="14"/>
@@ -1027,10 +1033,13 @@
       <c r="K11" t="b">
         <v>1</v>
       </c>
+      <c r="M11" t="b">
+        <v>1</v>
+      </c>
       <c r="P11" s="9"/>
       <c r="Q11" s="10">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="R11" s="13"/>
       <c r="S11" s="14"/>
@@ -1184,10 +1193,13 @@
       <c r="L17" t="b">
         <v>1</v>
       </c>
+      <c r="M17" t="b">
+        <v>1</v>
+      </c>
       <c r="P17" s="9"/>
       <c r="Q17" s="10">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="R17" s="13"/>
       <c r="S17" s="14"/>
@@ -1226,10 +1238,13 @@
       <c r="L18" t="b">
         <v>1</v>
       </c>
+      <c r="M18" t="b">
+        <v>1</v>
+      </c>
       <c r="P18" s="9"/>
       <c r="Q18" s="10">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="R18" s="13"/>
       <c r="S18" s="14"/>
@@ -1317,10 +1332,13 @@
       <c r="L21" t="b">
         <v>1</v>
       </c>
+      <c r="M21" t="b">
+        <v>1</v>
+      </c>
       <c r="P21" s="9"/>
       <c r="Q21" s="10">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="R21" s="13"/>
       <c r="S21" s="14"/>
@@ -1412,10 +1430,13 @@
       <c r="E25" t="b">
         <v>1</v>
       </c>
+      <c r="M25" t="b">
+        <v>1</v>
+      </c>
       <c r="P25" s="9"/>
       <c r="Q25" s="10">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="R25" s="13"/>
       <c r="S25" s="14"/>
@@ -1503,10 +1524,13 @@
       <c r="L28" t="b">
         <v>1</v>
       </c>
+      <c r="M28" t="b">
+        <v>1</v>
+      </c>
       <c r="P28" s="9"/>
       <c r="Q28" s="10">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="R28" s="13"/>
       <c r="S28" s="14"/>
@@ -1721,10 +1745,13 @@
       <c r="L36" t="b">
         <v>1</v>
       </c>
+      <c r="M36" t="b">
+        <v>1</v>
+      </c>
       <c r="P36" s="9"/>
       <c r="Q36" s="10">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="R36" s="13"/>
       <c r="S36" s="14"/>
@@ -1763,10 +1790,13 @@
       <c r="L37" t="b">
         <v>1</v>
       </c>
+      <c r="M37" t="b">
+        <v>1</v>
+      </c>
       <c r="P37" s="9"/>
       <c r="Q37" s="10">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="R37" s="13"/>
       <c r="S37" s="14"/>
@@ -1861,10 +1891,13 @@
       <c r="E41" t="b">
         <v>1</v>
       </c>
+      <c r="M41" t="b">
+        <v>1</v>
+      </c>
       <c r="P41" s="9"/>
       <c r="Q41" s="10">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R41" s="13"/>
       <c r="S41" s="14"/>
@@ -1892,10 +1925,13 @@
       <c r="L42" t="b">
         <v>1</v>
       </c>
+      <c r="M42" t="b">
+        <v>1</v>
+      </c>
       <c r="P42" s="9"/>
       <c r="Q42" s="10">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="R42" s="13"/>
       <c r="S42" s="14"/>
@@ -1992,10 +2028,13 @@
       <c r="L46" t="b">
         <v>1</v>
       </c>
+      <c r="M46" t="b">
+        <v>1</v>
+      </c>
       <c r="P46" s="9"/>
       <c r="Q46" s="10">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="R46" s="13"/>
       <c r="S46" s="14"/>

</xml_diff>

<commit_message>
lab 14.12.2023 - desenare maps + inceput de gasire path
</commit_message>
<xml_diff>
--- a/MetodeAvansate/Prezenta.xlsx
+++ b/MetodeAvansate/Prezenta.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\remus\Documents\GitHub\Facultate_2023\MetodeAvansate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4933CF7-AA69-4E3E-A9DC-F201F6C8D9CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6A55F7B-AA25-48B7-AEE6-865994F70E86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -732,8 +732,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:S47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="M11" sqref="M11"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="M24" sqref="M24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
@@ -927,10 +927,13 @@
       <c r="K7" t="b">
         <v>1</v>
       </c>
+      <c r="M7" t="b">
+        <v>1</v>
+      </c>
       <c r="P7" s="9"/>
       <c r="Q7" s="10">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="R7" s="13"/>
       <c r="S7" s="14"/>
@@ -971,10 +974,13 @@
       <c r="I9" t="b">
         <v>1</v>
       </c>
+      <c r="M9" t="b">
+        <v>1</v>
+      </c>
       <c r="P9" s="9"/>
       <c r="Q9" s="10">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="R9" s="13"/>
       <c r="S9" s="14"/>
@@ -1118,10 +1124,13 @@
       <c r="I15" t="b">
         <v>1</v>
       </c>
+      <c r="M15" t="b">
+        <v>1</v>
+      </c>
       <c r="P15" s="9"/>
       <c r="Q15" s="10">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="R15" s="13"/>
       <c r="S15" s="14"/>
@@ -1151,10 +1160,13 @@
       <c r="J16" t="b">
         <v>1</v>
       </c>
+      <c r="M16" t="b">
+        <v>1</v>
+      </c>
       <c r="P16" s="9"/>
       <c r="Q16" s="10">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="R16" s="13"/>
       <c r="S16" s="14"/>
@@ -1363,10 +1375,13 @@
       <c r="L22" t="b">
         <v>1</v>
       </c>
+      <c r="M22" t="b">
+        <v>1</v>
+      </c>
       <c r="P22" s="9"/>
       <c r="Q22" s="10">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="R22" s="13"/>
       <c r="S22" s="14"/>
@@ -1482,10 +1497,13 @@
       <c r="J27" t="b">
         <v>1</v>
       </c>
+      <c r="M27" t="b">
+        <v>1</v>
+      </c>
       <c r="P27" s="9"/>
       <c r="Q27" s="10">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="R27" s="13"/>
       <c r="S27" s="14"/>
@@ -1628,10 +1646,13 @@
       <c r="K31" t="b">
         <v>1</v>
       </c>
+      <c r="M31" t="b">
+        <v>1</v>
+      </c>
       <c r="P31" s="9"/>
       <c r="Q31" s="10">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="R31" s="13"/>
       <c r="S31" s="14"/>
@@ -1703,10 +1724,13 @@
       <c r="I35" t="b">
         <v>1</v>
       </c>
+      <c r="M35" t="b">
+        <v>1</v>
+      </c>
       <c r="P35" s="9"/>
       <c r="Q35" s="10">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="R35" s="13"/>
       <c r="S35" s="14"/>
@@ -1842,10 +1866,13 @@
       <c r="J39" t="b">
         <v>1</v>
       </c>
+      <c r="M39" t="b">
+        <v>1</v>
+      </c>
       <c r="P39" s="9"/>
       <c r="Q39" s="10">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="R39" s="13"/>
       <c r="S39" s="14"/>
@@ -1944,10 +1971,13 @@
       <c r="J43" t="b">
         <v>1</v>
       </c>
+      <c r="M43" t="b">
+        <v>1</v>
+      </c>
       <c r="P43" s="9"/>
       <c r="Q43" s="10">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R43" s="13"/>
       <c r="S43" s="14"/>
@@ -1969,10 +1999,13 @@
       <c r="J44" t="b">
         <v>1</v>
       </c>
+      <c r="M44" t="b">
+        <v>1</v>
+      </c>
       <c r="P44" s="9"/>
       <c r="Q44" s="10">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="R44" s="13"/>
       <c r="S44" s="14"/>
@@ -2000,10 +2033,13 @@
       <c r="I45" t="b">
         <v>1</v>
       </c>
+      <c r="M45" t="b">
+        <v>1</v>
+      </c>
       <c r="P45" s="9"/>
       <c r="Q45" s="10">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="R45" s="13"/>
       <c r="S45" s="14"/>

</xml_diff>

<commit_message>
forgot 2 saved files
</commit_message>
<xml_diff>
--- a/MetodeAvansate/Prezenta.xlsx
+++ b/MetodeAvansate/Prezenta.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\remus\Documents\GitHub\Facultate_2023\MetodeAvansate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6A55F7B-AA25-48B7-AEE6-865994F70E86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DB42D6D-3997-4B9A-9CDF-5F9458045F4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -732,8 +732,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:S47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="M24" sqref="M24"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="O6" sqref="O6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
@@ -1020,10 +1020,13 @@
       <c r="M10" t="b">
         <v>1</v>
       </c>
+      <c r="N10" t="b">
+        <v>1</v>
+      </c>
       <c r="P10" s="9"/>
       <c r="Q10" s="10">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="R10" s="13"/>
       <c r="S10" s="14"/>
@@ -1042,10 +1045,13 @@
       <c r="M11" t="b">
         <v>1</v>
       </c>
+      <c r="N11" t="b">
+        <v>1</v>
+      </c>
       <c r="P11" s="9"/>
       <c r="Q11" s="10">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="R11" s="13"/>
       <c r="S11" s="14"/>
@@ -1253,10 +1259,13 @@
       <c r="M18" t="b">
         <v>1</v>
       </c>
+      <c r="N18" t="b">
+        <v>1</v>
+      </c>
       <c r="P18" s="9"/>
       <c r="Q18" s="10">
         <f t="shared" si="0"/>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="R18" s="13"/>
       <c r="S18" s="14"/>
@@ -1347,10 +1356,13 @@
       <c r="M21" t="b">
         <v>1</v>
       </c>
+      <c r="N21" t="b">
+        <v>1</v>
+      </c>
       <c r="P21" s="9"/>
       <c r="Q21" s="10">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="R21" s="13"/>
       <c r="S21" s="14"/>
@@ -1448,10 +1460,13 @@
       <c r="M25" t="b">
         <v>1</v>
       </c>
+      <c r="N25" t="b">
+        <v>1</v>
+      </c>
       <c r="P25" s="9"/>
       <c r="Q25" s="10">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="R25" s="13"/>
       <c r="S25" s="14"/>
@@ -1545,10 +1560,13 @@
       <c r="M28" t="b">
         <v>1</v>
       </c>
+      <c r="N28" t="b">
+        <v>1</v>
+      </c>
       <c r="P28" s="9"/>
       <c r="Q28" s="10">
         <f t="shared" si="0"/>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="R28" s="13"/>
       <c r="S28" s="14"/>
@@ -1772,10 +1790,13 @@
       <c r="M36" t="b">
         <v>1</v>
       </c>
+      <c r="N36" t="b">
+        <v>1</v>
+      </c>
       <c r="P36" s="9"/>
       <c r="Q36" s="10">
         <f t="shared" si="0"/>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="R36" s="13"/>
       <c r="S36" s="14"/>
@@ -1817,10 +1838,13 @@
       <c r="M37" t="b">
         <v>1</v>
       </c>
+      <c r="N37" t="b">
+        <v>1</v>
+      </c>
       <c r="P37" s="9"/>
       <c r="Q37" s="10">
         <f t="shared" si="0"/>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="R37" s="13"/>
       <c r="S37" s="14"/>
@@ -1921,10 +1945,13 @@
       <c r="M41" t="b">
         <v>1</v>
       </c>
+      <c r="N41" t="b">
+        <v>1</v>
+      </c>
       <c r="P41" s="9"/>
       <c r="Q41" s="10">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="R41" s="13"/>
       <c r="S41" s="14"/>

</xml_diff>

<commit_message>
core module, base layout, home and login modules, routing
</commit_message>
<xml_diff>
--- a/MetodeAvansate/Prezenta.xlsx
+++ b/MetodeAvansate/Prezenta.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\remus\Documents\GitHub\Facultate_2023\MetodeAvansate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3357CB8-5546-4D06-B682-C3A904B657FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5368C934-6420-4EFB-8C41-5F2B91B4ECB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -733,7 +733,7 @@
   <dimension ref="B2:S47"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A20" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="L34" sqref="L34"/>
+      <selection activeCell="O32" sqref="O32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>

</xml_diff>

<commit_message>
notele de pana acum
</commit_message>
<xml_diff>
--- a/MetodeAvansate/Prezenta.xlsx
+++ b/MetodeAvansate/Prezenta.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\remus\Documents\GitHub\Facultate_2023\MetodeAvansate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5368C934-6420-4EFB-8C41-5F2B91B4ECB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A33003D0-AD2E-4662-91B8-C653308CB8F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="78">
   <si>
     <t>Nume Prenume</t>
   </si>
@@ -209,6 +209,51 @@
   </si>
   <si>
     <t>Pecherle George</t>
+  </si>
+  <si>
+    <t>Expense Tracker</t>
+  </si>
+  <si>
+    <t>Market Place</t>
+  </si>
+  <si>
+    <t>Ceva Site</t>
+  </si>
+  <si>
+    <t>Social Media App</t>
+  </si>
+  <si>
+    <t>Series Library</t>
+  </si>
+  <si>
+    <t>Proiect Grafuri</t>
+  </si>
+  <si>
+    <t>Invoice App</t>
+  </si>
+  <si>
+    <t>Site Restaurant</t>
+  </si>
+  <si>
+    <t>Ilisei Rares</t>
+  </si>
+  <si>
+    <t>Mihaila Marian</t>
+  </si>
+  <si>
+    <t>Site ProPc</t>
+  </si>
+  <si>
+    <t>Site SwiftSupp</t>
+  </si>
+  <si>
+    <t>Site MusicStreaming</t>
+  </si>
+  <si>
+    <t>Site Social</t>
+  </si>
+  <si>
+    <t>Site Dressa</t>
   </si>
 </sst>
 </file>
@@ -402,7 +447,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -445,6 +490,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -730,17 +778,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:S47"/>
+  <dimension ref="B2:S49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="O32" sqref="O32"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="T48" sqref="T48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="2.6640625" customWidth="1"/>
-    <col min="2" max="2" width="20.88671875" customWidth="1"/>
-    <col min="18" max="18" width="15.33203125" customWidth="1"/>
+    <col min="1" max="1" width="2.7109375" customWidth="1"/>
+    <col min="2" max="2" width="20.85546875" customWidth="1"/>
+    <col min="18" max="18" width="25.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:19">
@@ -823,14 +871,20 @@
       <c r="L3" s="4"/>
       <c r="M3" s="4"/>
       <c r="N3" s="4"/>
-      <c r="O3" s="4"/>
+      <c r="O3" s="4" t="b">
+        <v>1</v>
+      </c>
       <c r="P3" s="8"/>
       <c r="Q3" s="10">
-        <f t="shared" ref="Q3:Q47" si="0">C3+D3+E3+F3+G3+H3+I3+J3+K3+L3+M3+N3+O3+P3</f>
-        <v>4</v>
-      </c>
-      <c r="R3" s="11"/>
-      <c r="S3" s="12"/>
+        <f t="shared" ref="Q3:Q49" si="0">C3+D3+E3+F3+G3+H3+I3+J3+K3+L3+M3+N3+O3+P3</f>
+        <v>5</v>
+      </c>
+      <c r="R3" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="S3" s="12">
+        <v>9</v>
+      </c>
     </row>
     <row r="4" spans="2:19">
       <c r="B4" s="16" t="s">
@@ -846,7 +900,9 @@
         <v>1</v>
       </c>
       <c r="R4" s="13"/>
-      <c r="S4" s="14"/>
+      <c r="S4" s="14">
+        <v>5</v>
+      </c>
     </row>
     <row r="5" spans="2:19">
       <c r="B5" s="16" t="s">
@@ -862,7 +918,9 @@
         <v>1</v>
       </c>
       <c r="R5" s="13"/>
-      <c r="S5" s="14"/>
+      <c r="S5" s="14">
+        <v>5</v>
+      </c>
     </row>
     <row r="6" spans="2:19">
       <c r="B6" s="16" t="s">
@@ -899,13 +957,22 @@
       <c r="M6" t="b">
         <v>1</v>
       </c>
-      <c r="P6" s="9"/>
+      <c r="O6" t="b">
+        <v>1</v>
+      </c>
+      <c r="P6" s="9" t="b">
+        <v>1</v>
+      </c>
       <c r="Q6" s="10">
         <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="R6" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="S6" s="14">
         <v>10</v>
       </c>
-      <c r="R6" s="13"/>
-      <c r="S6" s="14"/>
     </row>
     <row r="7" spans="2:19">
       <c r="B7" s="16" t="s">
@@ -933,13 +1000,18 @@
       <c r="N7" t="b">
         <v>1</v>
       </c>
+      <c r="O7" t="b">
+        <v>1</v>
+      </c>
       <c r="P7" s="9"/>
       <c r="Q7" s="10">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="R7" s="13"/>
-      <c r="S7" s="14"/>
+      <c r="S7" s="14">
+        <v>6</v>
+      </c>
     </row>
     <row r="8" spans="2:19">
       <c r="B8" s="16" t="s">
@@ -964,7 +1036,9 @@
         <v>4</v>
       </c>
       <c r="R8" s="13"/>
-      <c r="S8" s="14"/>
+      <c r="S8" s="14">
+        <v>6</v>
+      </c>
     </row>
     <row r="9" spans="2:19">
       <c r="B9" s="16" t="s">
@@ -980,13 +1054,20 @@
       <c r="M9" t="b">
         <v>1</v>
       </c>
-      <c r="P9" s="9"/>
+      <c r="O9" t="b">
+        <v>1</v>
+      </c>
+      <c r="P9" s="9" t="b">
+        <v>1</v>
+      </c>
       <c r="Q9" s="10">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="R9" s="13"/>
-      <c r="S9" s="14"/>
+      <c r="S9" s="14">
+        <v>6</v>
+      </c>
     </row>
     <row r="10" spans="2:19">
       <c r="B10" s="16" t="s">
@@ -1026,13 +1107,22 @@
       <c r="N10" t="b">
         <v>1</v>
       </c>
-      <c r="P10" s="9"/>
+      <c r="O10" t="b">
+        <v>1</v>
+      </c>
+      <c r="P10" s="9" t="b">
+        <v>1</v>
+      </c>
       <c r="Q10" s="10">
         <f t="shared" si="0"/>
-        <v>11</v>
-      </c>
-      <c r="R10" s="13"/>
-      <c r="S10" s="14"/>
+        <v>13</v>
+      </c>
+      <c r="R10" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="S10" s="14">
+        <v>9</v>
+      </c>
     </row>
     <row r="11" spans="2:19">
       <c r="B11" s="16" t="s">
@@ -1057,7 +1147,9 @@
         <v>4</v>
       </c>
       <c r="R11" s="13"/>
-      <c r="S11" s="14"/>
+      <c r="S11" s="14">
+        <v>6</v>
+      </c>
     </row>
     <row r="12" spans="2:19">
       <c r="B12" s="16" t="s">
@@ -1073,7 +1165,9 @@
         <v>1</v>
       </c>
       <c r="R12" s="13"/>
-      <c r="S12" s="14"/>
+      <c r="S12" s="14">
+        <v>5</v>
+      </c>
     </row>
     <row r="13" spans="2:19">
       <c r="B13" s="16" t="s">
@@ -1091,7 +1185,9 @@
         <v>2</v>
       </c>
       <c r="R13" s="13"/>
-      <c r="S13" s="14"/>
+      <c r="S13" s="14">
+        <v>5</v>
+      </c>
     </row>
     <row r="14" spans="2:19">
       <c r="B14" s="16" t="s">
@@ -1106,7 +1202,9 @@
         <v>1</v>
       </c>
       <c r="R14" s="13"/>
-      <c r="S14" s="14"/>
+      <c r="S14" s="14">
+        <v>5</v>
+      </c>
     </row>
     <row r="15" spans="2:19">
       <c r="B15" s="16" t="s">
@@ -1136,13 +1234,22 @@
       <c r="M15" t="b">
         <v>1</v>
       </c>
-      <c r="P15" s="9"/>
+      <c r="O15" t="b">
+        <v>1</v>
+      </c>
+      <c r="P15" s="9" t="b">
+        <v>1</v>
+      </c>
       <c r="Q15" s="10">
         <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="R15" s="13"/>
-      <c r="S15" s="14"/>
+        <v>10</v>
+      </c>
+      <c r="R15" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="S15" s="14">
+        <v>10</v>
+      </c>
     </row>
     <row r="16" spans="2:19">
       <c r="B16" s="16" t="s">
@@ -1172,13 +1279,22 @@
       <c r="M16" t="b">
         <v>1</v>
       </c>
-      <c r="P16" s="9"/>
+      <c r="O16" t="b">
+        <v>1</v>
+      </c>
+      <c r="P16" s="9" t="b">
+        <v>1</v>
+      </c>
       <c r="Q16" s="10">
         <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="R16" s="13"/>
-      <c r="S16" s="14"/>
+        <v>10</v>
+      </c>
+      <c r="R16" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="S16" s="14">
+        <v>10</v>
+      </c>
     </row>
     <row r="17" spans="2:19">
       <c r="B17" s="16" t="s">
@@ -1220,13 +1336,22 @@
       <c r="N17" t="b">
         <v>1</v>
       </c>
-      <c r="P17" s="9"/>
+      <c r="O17" t="b">
+        <v>1</v>
+      </c>
+      <c r="P17" s="9" t="b">
+        <v>1</v>
+      </c>
       <c r="Q17" s="10">
         <f t="shared" si="0"/>
-        <v>12</v>
-      </c>
-      <c r="R17" s="13"/>
-      <c r="S17" s="14"/>
+        <v>14</v>
+      </c>
+      <c r="R17" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="S17" s="14">
+        <v>10</v>
+      </c>
     </row>
     <row r="18" spans="2:19">
       <c r="B18" s="16" t="s">
@@ -1268,13 +1393,22 @@
       <c r="N18" t="b">
         <v>1</v>
       </c>
-      <c r="P18" s="9"/>
+      <c r="O18" t="b">
+        <v>1</v>
+      </c>
+      <c r="P18" s="9" t="b">
+        <v>1</v>
+      </c>
       <c r="Q18" s="10">
         <f t="shared" si="0"/>
-        <v>12</v>
-      </c>
-      <c r="R18" s="13"/>
-      <c r="S18" s="14"/>
+        <v>14</v>
+      </c>
+      <c r="R18" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="S18" s="14">
+        <v>10</v>
+      </c>
     </row>
     <row r="19" spans="2:19">
       <c r="B19" s="16" t="s">
@@ -1304,13 +1438,20 @@
       <c r="N19" t="b">
         <v>1</v>
       </c>
+      <c r="O19" t="b">
+        <v>1</v>
+      </c>
       <c r="P19" s="9"/>
       <c r="Q19" s="10">
         <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="R19" s="13"/>
-      <c r="S19" s="14"/>
+        <v>9</v>
+      </c>
+      <c r="R19" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="S19" s="14">
+        <v>10</v>
+      </c>
     </row>
     <row r="20" spans="2:19">
       <c r="B20" s="16" t="s">
@@ -1323,13 +1464,22 @@
       <c r="I20" t="b">
         <v>1</v>
       </c>
-      <c r="P20" s="9"/>
+      <c r="O20" t="b">
+        <v>1</v>
+      </c>
+      <c r="P20" s="9" t="b">
+        <v>1</v>
+      </c>
       <c r="Q20" s="10">
         <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="R20" s="13"/>
-      <c r="S20" s="14"/>
+        <v>4</v>
+      </c>
+      <c r="R20" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="S20" s="14">
+        <v>10</v>
+      </c>
     </row>
     <row r="21" spans="2:19">
       <c r="B21" s="16" t="s">
@@ -1368,13 +1518,19 @@
       <c r="N21" t="b">
         <v>1</v>
       </c>
-      <c r="P21" s="9"/>
+      <c r="P21" s="9" t="b">
+        <v>1</v>
+      </c>
       <c r="Q21" s="10">
         <f t="shared" si="0"/>
-        <v>11</v>
-      </c>
-      <c r="R21" s="13"/>
-      <c r="S21" s="14"/>
+        <v>12</v>
+      </c>
+      <c r="R21" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="S21" s="14">
+        <v>10</v>
+      </c>
     </row>
     <row r="22" spans="2:19">
       <c r="B22" s="16" t="s">
@@ -1399,13 +1555,19 @@
       <c r="M22" t="b">
         <v>1</v>
       </c>
-      <c r="P22" s="9"/>
+      <c r="P22" s="9" t="b">
+        <v>1</v>
+      </c>
       <c r="Q22" s="10">
         <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="R22" s="13"/>
-      <c r="S22" s="14"/>
+        <v>7</v>
+      </c>
+      <c r="R22" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="S22" s="14">
+        <v>8</v>
+      </c>
     </row>
     <row r="23" spans="2:19">
       <c r="B23" s="16" t="s">
@@ -1432,13 +1594,20 @@
       <c r="N23" t="b">
         <v>1</v>
       </c>
+      <c r="O23" t="b">
+        <v>1</v>
+      </c>
       <c r="P23" s="9"/>
       <c r="Q23" s="10">
         <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="R23" s="13"/>
-      <c r="S23" s="14"/>
+        <v>8</v>
+      </c>
+      <c r="R23" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="S23" s="14">
+        <v>10</v>
+      </c>
     </row>
     <row r="24" spans="2:19">
       <c r="B24" s="16" t="s">
@@ -1454,7 +1623,9 @@
         <v>1</v>
       </c>
       <c r="R24" s="13"/>
-      <c r="S24" s="14"/>
+      <c r="S24" s="14">
+        <v>5</v>
+      </c>
     </row>
     <row r="25" spans="2:19">
       <c r="B25" s="16" t="s">
@@ -1475,13 +1646,22 @@
       <c r="N25" t="b">
         <v>1</v>
       </c>
-      <c r="P25" s="9"/>
+      <c r="O25" t="b">
+        <v>1</v>
+      </c>
+      <c r="P25" s="9" t="b">
+        <v>1</v>
+      </c>
       <c r="Q25" s="10">
         <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="R25" s="13"/>
-      <c r="S25" s="14"/>
+        <v>7</v>
+      </c>
+      <c r="R25" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="S25" s="14">
+        <v>10</v>
+      </c>
     </row>
     <row r="26" spans="2:19">
       <c r="B26" s="16" t="s">
@@ -1490,13 +1670,22 @@
       <c r="C26" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="P26" s="9"/>
+      <c r="O26" t="b">
+        <v>1</v>
+      </c>
+      <c r="P26" s="9" t="b">
+        <v>1</v>
+      </c>
       <c r="Q26" s="10">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="R26" s="13"/>
-      <c r="S26" s="14"/>
+        <v>3</v>
+      </c>
+      <c r="R26" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="S26" s="14">
+        <v>8</v>
+      </c>
     </row>
     <row r="27" spans="2:19">
       <c r="B27" s="16" t="s">
@@ -1530,13 +1719,18 @@
       <c r="N27" t="b">
         <v>1</v>
       </c>
+      <c r="O27" t="b">
+        <v>1</v>
+      </c>
       <c r="P27" s="9"/>
       <c r="Q27" s="10">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="R27" s="13"/>
-      <c r="S27" s="14"/>
+      <c r="S27" s="14">
+        <v>6</v>
+      </c>
     </row>
     <row r="28" spans="2:19">
       <c r="B28" s="16" t="s">
@@ -1578,13 +1772,22 @@
       <c r="N28" t="b">
         <v>1</v>
       </c>
-      <c r="P28" s="9"/>
+      <c r="O28" t="b">
+        <v>1</v>
+      </c>
+      <c r="P28" s="9" t="b">
+        <v>1</v>
+      </c>
       <c r="Q28" s="10">
         <f t="shared" si="0"/>
-        <v>12</v>
-      </c>
-      <c r="R28" s="13"/>
-      <c r="S28" s="14"/>
+        <v>14</v>
+      </c>
+      <c r="R28" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="S28" s="14">
+        <v>9</v>
+      </c>
     </row>
     <row r="29" spans="2:19">
       <c r="B29" s="16" t="s">
@@ -1612,13 +1815,22 @@
       <c r="K29" t="b">
         <v>1</v>
       </c>
-      <c r="P29" s="9"/>
+      <c r="O29" t="b">
+        <v>1</v>
+      </c>
+      <c r="P29" s="9" t="b">
+        <v>1</v>
+      </c>
       <c r="Q29" s="10">
         <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="R29" s="13"/>
-      <c r="S29" s="14"/>
+        <v>9</v>
+      </c>
+      <c r="R29" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="S29" s="14">
+        <v>9</v>
+      </c>
     </row>
     <row r="30" spans="2:19">
       <c r="B30" s="16" t="s">
@@ -1654,13 +1866,20 @@
       <c r="N30" t="b">
         <v>1</v>
       </c>
+      <c r="O30" t="b">
+        <v>1</v>
+      </c>
       <c r="P30" s="9"/>
       <c r="Q30" s="10">
         <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="R30" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="S30" s="14">
         <v>10</v>
       </c>
-      <c r="R30" s="13"/>
-      <c r="S30" s="14"/>
     </row>
     <row r="31" spans="2:19">
       <c r="B31" s="16" t="s">
@@ -1685,13 +1904,20 @@
       <c r="M31" t="b">
         <v>1</v>
       </c>
+      <c r="O31" t="b">
+        <v>1</v>
+      </c>
       <c r="P31" s="9"/>
       <c r="Q31" s="10">
         <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="R31" s="13"/>
-      <c r="S31" s="14"/>
+        <v>7</v>
+      </c>
+      <c r="R31" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="S31" s="14">
+        <v>10</v>
+      </c>
     </row>
     <row r="32" spans="2:19">
       <c r="B32" s="16" t="s">
@@ -1707,7 +1933,9 @@
         <v>1</v>
       </c>
       <c r="R32" s="13"/>
-      <c r="S32" s="14"/>
+      <c r="S32" s="14">
+        <v>5</v>
+      </c>
     </row>
     <row r="33" spans="2:19">
       <c r="B33" s="16" t="s">
@@ -1720,13 +1948,22 @@
       <c r="N33" t="b">
         <v>1</v>
       </c>
-      <c r="P33" s="9"/>
+      <c r="O33" t="b">
+        <v>1</v>
+      </c>
+      <c r="P33" s="9" t="b">
+        <v>1</v>
+      </c>
       <c r="Q33" s="10">
         <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="R33" s="13"/>
-      <c r="S33" s="14"/>
+        <v>4</v>
+      </c>
+      <c r="R33" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="S33" s="14">
+        <v>10</v>
+      </c>
     </row>
     <row r="34" spans="2:19">
       <c r="B34" s="16" t="s">
@@ -1744,13 +1981,22 @@
       <c r="I34" t="b">
         <v>1</v>
       </c>
-      <c r="P34" s="9"/>
+      <c r="O34" t="b">
+        <v>1</v>
+      </c>
+      <c r="P34" s="9" t="b">
+        <v>1</v>
+      </c>
       <c r="Q34" s="10">
         <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="R34" s="13"/>
-      <c r="S34" s="14"/>
+        <v>6</v>
+      </c>
+      <c r="R34" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="S34" s="14">
+        <v>9</v>
+      </c>
     </row>
     <row r="35" spans="2:19">
       <c r="B35" s="16" t="s">
@@ -1769,13 +2015,20 @@
       <c r="N35" t="b">
         <v>1</v>
       </c>
+      <c r="O35" t="b">
+        <v>1</v>
+      </c>
       <c r="P35" s="9"/>
       <c r="Q35" s="10">
         <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="R35" s="13"/>
-      <c r="S35" s="14"/>
+        <v>5</v>
+      </c>
+      <c r="R35" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="S35" s="14">
+        <v>9</v>
+      </c>
     </row>
     <row r="36" spans="2:19">
       <c r="B36" s="16" t="s">
@@ -1817,13 +2070,20 @@
       <c r="N36" t="b">
         <v>1</v>
       </c>
+      <c r="O36" t="b">
+        <v>1</v>
+      </c>
       <c r="P36" s="9"/>
       <c r="Q36" s="10">
         <f t="shared" si="0"/>
-        <v>12</v>
-      </c>
-      <c r="R36" s="13"/>
-      <c r="S36" s="14"/>
+        <v>13</v>
+      </c>
+      <c r="R36" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="S36" s="14">
+        <v>10</v>
+      </c>
     </row>
     <row r="37" spans="2:19">
       <c r="B37" s="16" t="s">
@@ -1865,13 +2125,20 @@
       <c r="N37" t="b">
         <v>1</v>
       </c>
-      <c r="P37" s="9"/>
+      <c r="O37" t="b">
+        <v>1</v>
+      </c>
+      <c r="P37" s="9" t="b">
+        <v>1</v>
+      </c>
       <c r="Q37" s="10">
         <f t="shared" si="0"/>
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="R37" s="13"/>
-      <c r="S37" s="14"/>
+      <c r="S37" s="14">
+        <v>6</v>
+      </c>
     </row>
     <row r="38" spans="2:19">
       <c r="B38" s="16" t="s">
@@ -1889,13 +2156,19 @@
       <c r="N38" t="b">
         <v>1</v>
       </c>
-      <c r="P38" s="9"/>
+      <c r="P38" s="9" t="b">
+        <v>1</v>
+      </c>
       <c r="Q38" s="10">
         <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="R38" s="13"/>
-      <c r="S38" s="14"/>
+        <v>5</v>
+      </c>
+      <c r="R38" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="S38" s="14">
+        <v>9</v>
+      </c>
     </row>
     <row r="39" spans="2:19">
       <c r="B39" s="16" t="s">
@@ -1920,13 +2193,20 @@
       <c r="M39" t="b">
         <v>1</v>
       </c>
+      <c r="O39" t="b">
+        <v>1</v>
+      </c>
       <c r="P39" s="9"/>
       <c r="Q39" s="10">
         <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="R39" s="13"/>
-      <c r="S39" s="14"/>
+        <v>7</v>
+      </c>
+      <c r="R39" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="S39" s="14">
+        <v>10</v>
+      </c>
     </row>
     <row r="40" spans="2:19">
       <c r="B40" s="16" t="s">
@@ -1953,13 +2233,19 @@
       <c r="J40" t="b">
         <v>1</v>
       </c>
-      <c r="P40" s="9"/>
+      <c r="P40" s="9" t="b">
+        <v>1</v>
+      </c>
       <c r="Q40" s="10">
         <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="R40" s="13"/>
-      <c r="S40" s="14"/>
+        <v>8</v>
+      </c>
+      <c r="R40" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="S40" s="14">
+        <v>9</v>
+      </c>
     </row>
     <row r="41" spans="2:19">
       <c r="B41" s="16" t="s">
@@ -1975,13 +2261,20 @@
       <c r="N41" t="b">
         <v>1</v>
       </c>
-      <c r="P41" s="9"/>
+      <c r="O41" t="b">
+        <v>1</v>
+      </c>
+      <c r="P41" s="9" t="b">
+        <v>1</v>
+      </c>
       <c r="Q41" s="10">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="R41" s="13"/>
-      <c r="S41" s="14"/>
+      <c r="S41" s="14">
+        <v>6</v>
+      </c>
     </row>
     <row r="42" spans="2:19">
       <c r="B42" s="16" t="s">
@@ -2009,13 +2302,22 @@
       <c r="M42" t="b">
         <v>1</v>
       </c>
-      <c r="P42" s="9"/>
+      <c r="O42" t="b">
+        <v>1</v>
+      </c>
+      <c r="P42" s="9" t="b">
+        <v>1</v>
+      </c>
       <c r="Q42" s="10">
         <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="R42" s="13"/>
-      <c r="S42" s="14"/>
+        <v>9</v>
+      </c>
+      <c r="R42" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="S42" s="14">
+        <v>8</v>
+      </c>
     </row>
     <row r="43" spans="2:19">
       <c r="B43" s="16" t="s">
@@ -2028,13 +2330,18 @@
       <c r="M43" t="b">
         <v>1</v>
       </c>
+      <c r="O43" t="b">
+        <v>1</v>
+      </c>
       <c r="P43" s="9"/>
       <c r="Q43" s="10">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="R43" s="13"/>
-      <c r="S43" s="14"/>
+      <c r="S43" s="14">
+        <v>5</v>
+      </c>
     </row>
     <row r="44" spans="2:19">
       <c r="B44" s="17" t="s">
@@ -2056,13 +2363,22 @@
       <c r="M44" t="b">
         <v>1</v>
       </c>
-      <c r="P44" s="9"/>
+      <c r="O44" t="b">
+        <v>1</v>
+      </c>
+      <c r="P44" s="9" t="b">
+        <v>1</v>
+      </c>
       <c r="Q44" s="10">
         <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="R44" s="13"/>
-      <c r="S44" s="14"/>
+        <v>7</v>
+      </c>
+      <c r="R44" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="S44" s="14">
+        <v>9</v>
+      </c>
     </row>
     <row r="45" spans="2:19">
       <c r="B45" s="16" t="s">
@@ -2090,13 +2406,20 @@
       <c r="M45" t="b">
         <v>1</v>
       </c>
+      <c r="O45" t="b">
+        <v>1</v>
+      </c>
       <c r="P45" s="9"/>
       <c r="Q45" s="10">
         <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="R45" s="13"/>
-      <c r="S45" s="14"/>
+        <v>8</v>
+      </c>
+      <c r="R45" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="S45" s="14">
+        <v>10</v>
+      </c>
     </row>
     <row r="46" spans="2:19">
       <c r="B46" s="16" t="s">
@@ -2121,13 +2444,19 @@
       <c r="M46" t="b">
         <v>1</v>
       </c>
-      <c r="P46" s="9"/>
+      <c r="P46" s="9" t="b">
+        <v>1</v>
+      </c>
       <c r="Q46" s="10">
         <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="R46" s="13"/>
-      <c r="S46" s="14"/>
+        <v>7</v>
+      </c>
+      <c r="R46" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="S46" s="14">
+        <v>10</v>
+      </c>
     </row>
     <row r="47" spans="2:19">
       <c r="B47" s="16" t="s">
@@ -2158,19 +2487,61 @@
       <c r="M47" s="7"/>
       <c r="N47" s="7"/>
       <c r="O47" s="7"/>
-      <c r="P47" s="7"/>
+      <c r="P47" s="7" t="b">
+        <v>1</v>
+      </c>
       <c r="Q47" s="18">
         <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="R47" s="19"/>
-      <c r="S47" s="15"/>
+        <v>7</v>
+      </c>
+      <c r="R47" s="19" t="s">
+        <v>76</v>
+      </c>
+      <c r="S47" s="15">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="48" spans="2:19">
+      <c r="B48" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="P48" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q48" s="18">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="R48" t="s">
+        <v>68</v>
+      </c>
+      <c r="S48" s="20">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="49" spans="2:19">
+      <c r="B49" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="P49" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q49" s="18">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="R49" t="s">
+        <v>68</v>
+      </c>
+      <c r="S49">
+        <v>7</v>
+      </c>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:S47">
     <sortCondition ref="B47"/>
   </sortState>
-  <conditionalFormatting sqref="Q3:Q47">
+  <conditionalFormatting sqref="Q3:Q49">
     <cfRule type="cellIs" dxfId="0" priority="2" operator="lessThan">
       <formula>4</formula>
     </cfRule>

</xml_diff>

<commit_message>
note finale + 5 tije
</commit_message>
<xml_diff>
--- a/MetodeAvansate/Prezenta.xlsx
+++ b/MetodeAvansate/Prezenta.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\remus\Documents\GitHub\Facultate_2023\MetodeAvansate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A33003D0-AD2E-4662-91B8-C653308CB8F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E1CE87D-101C-4B60-8944-97DA3CFF7BD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="80">
   <si>
     <t>Nume Prenume</t>
   </si>
@@ -254,6 +254,12 @@
   </si>
   <si>
     <t>Site Dressa</t>
+  </si>
+  <si>
+    <t>Vaida David</t>
+  </si>
+  <si>
+    <t>Site Rest Vegan</t>
   </si>
 </sst>
 </file>
@@ -447,7 +453,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -486,13 +492,17 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -778,17 +788,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:S49"/>
+  <dimension ref="B2:S50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="T48" sqref="T48"/>
+    <sheetView tabSelected="1" topLeftCell="A20" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="T38" sqref="T38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="2.7109375" customWidth="1"/>
-    <col min="2" max="2" width="20.85546875" customWidth="1"/>
-    <col min="18" max="18" width="25.140625" customWidth="1"/>
+    <col min="1" max="1" width="2.6640625" customWidth="1"/>
+    <col min="2" max="2" width="20.88671875" customWidth="1"/>
+    <col min="18" max="18" width="25.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:19">
@@ -876,7 +886,7 @@
       </c>
       <c r="P3" s="8"/>
       <c r="Q3" s="10">
-        <f t="shared" ref="Q3:Q49" si="0">C3+D3+E3+F3+G3+H3+I3+J3+K3+L3+M3+N3+O3+P3</f>
+        <f t="shared" ref="Q3:Q50" si="0">C3+D3+E3+F3+G3+H3+I3+J3+K3+L3+M3+N3+O3+P3</f>
         <v>5</v>
       </c>
       <c r="R3" s="11" t="s">
@@ -1253,52 +1263,26 @@
     </row>
     <row r="16" spans="2:19">
       <c r="B16" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="C16" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="D16" t="b">
-        <v>1</v>
-      </c>
-      <c r="E16" t="b">
-        <v>1</v>
-      </c>
-      <c r="F16" t="b">
-        <v>1</v>
-      </c>
-      <c r="H16" t="b">
-        <v>1</v>
-      </c>
-      <c r="I16" t="b">
-        <v>1</v>
-      </c>
-      <c r="J16" t="b">
-        <v>1</v>
-      </c>
-      <c r="M16" t="b">
-        <v>1</v>
-      </c>
-      <c r="O16" t="b">
-        <v>1</v>
-      </c>
+        <v>71</v>
+      </c>
+      <c r="C16" s="5"/>
       <c r="P16" s="9" t="b">
         <v>1</v>
       </c>
       <c r="Q16" s="10">
         <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="R16" s="13" t="s">
-        <v>70</v>
+        <v>1</v>
+      </c>
+      <c r="R16" s="20" t="s">
+        <v>68</v>
       </c>
       <c r="S16" s="14">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="17" spans="2:19">
       <c r="B17" s="16" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C17" s="5" t="b">
         <v>1</v>
@@ -1312,9 +1296,6 @@
       <c r="F17" t="b">
         <v>1</v>
       </c>
-      <c r="G17" t="b">
-        <v>1</v>
-      </c>
       <c r="H17" t="b">
         <v>1</v>
       </c>
@@ -1324,18 +1305,9 @@
       <c r="J17" t="b">
         <v>1</v>
       </c>
-      <c r="K17" t="b">
-        <v>1</v>
-      </c>
-      <c r="L17" t="b">
-        <v>1</v>
-      </c>
       <c r="M17" t="b">
         <v>1</v>
       </c>
-      <c r="N17" t="b">
-        <v>1</v>
-      </c>
       <c r="O17" t="b">
         <v>1</v>
       </c>
@@ -1344,10 +1316,10 @@
       </c>
       <c r="Q17" s="10">
         <f t="shared" si="0"/>
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="R17" s="13" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="S17" s="14">
         <v>10</v>
@@ -1355,7 +1327,7 @@
     </row>
     <row r="18" spans="2:19">
       <c r="B18" s="16" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C18" s="5" t="b">
         <v>1</v>
@@ -1412,11 +1384,14 @@
     </row>
     <row r="19" spans="2:19">
       <c r="B19" s="16" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="C19" s="5" t="b">
         <v>1</v>
       </c>
+      <c r="D19" t="b">
+        <v>1</v>
+      </c>
       <c r="E19" t="b">
         <v>1</v>
       </c>
@@ -1429,25 +1404,36 @@
       <c r="H19" t="b">
         <v>1</v>
       </c>
+      <c r="I19" t="b">
+        <v>1</v>
+      </c>
       <c r="J19" t="b">
         <v>1</v>
       </c>
       <c r="K19" t="b">
         <v>1</v>
       </c>
+      <c r="L19" t="b">
+        <v>1</v>
+      </c>
+      <c r="M19" t="b">
+        <v>1</v>
+      </c>
       <c r="N19" t="b">
         <v>1</v>
       </c>
       <c r="O19" t="b">
         <v>1</v>
       </c>
-      <c r="P19" s="9"/>
+      <c r="P19" s="9" t="b">
+        <v>1</v>
+      </c>
       <c r="Q19" s="10">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="R19" s="13" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="S19" s="14">
         <v>10</v>
@@ -1455,27 +1441,42 @@
     </row>
     <row r="20" spans="2:19">
       <c r="B20" s="16" t="s">
-        <v>54</v>
-      </c>
-      <c r="C20" s="5"/>
+        <v>18</v>
+      </c>
+      <c r="C20" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="E20" t="b">
+        <v>1</v>
+      </c>
       <c r="F20" t="b">
         <v>1</v>
       </c>
-      <c r="I20" t="b">
+      <c r="G20" t="b">
+        <v>1</v>
+      </c>
+      <c r="H20" t="b">
+        <v>1</v>
+      </c>
+      <c r="J20" t="b">
+        <v>1</v>
+      </c>
+      <c r="K20" t="b">
+        <v>1</v>
+      </c>
+      <c r="N20" t="b">
         <v>1</v>
       </c>
       <c r="O20" t="b">
         <v>1</v>
       </c>
-      <c r="P20" s="9" t="b">
-        <v>1</v>
-      </c>
+      <c r="P20" s="9"/>
       <c r="Q20" s="10">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="R20" s="13" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="S20" s="14">
         <v>10</v>
@@ -1483,39 +1484,16 @@
     </row>
     <row r="21" spans="2:19">
       <c r="B21" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="C21" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="D21" t="b">
-        <v>1</v>
-      </c>
-      <c r="E21" t="b">
-        <v>1</v>
-      </c>
+        <v>54</v>
+      </c>
+      <c r="C21" s="5"/>
       <c r="F21" t="b">
         <v>1</v>
       </c>
-      <c r="G21" t="b">
-        <v>1</v>
-      </c>
-      <c r="H21" t="b">
-        <v>1</v>
-      </c>
       <c r="I21" t="b">
         <v>1</v>
       </c>
-      <c r="K21" t="b">
-        <v>1</v>
-      </c>
-      <c r="L21" t="b">
-        <v>1</v>
-      </c>
-      <c r="M21" t="b">
-        <v>1</v>
-      </c>
-      <c r="N21" t="b">
+      <c r="O21" t="b">
         <v>1</v>
       </c>
       <c r="P21" s="9" t="b">
@@ -1523,7 +1501,7 @@
       </c>
       <c r="Q21" s="10">
         <f t="shared" si="0"/>
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="R21" s="13" t="s">
         <v>68</v>
@@ -1534,9 +1512,14 @@
     </row>
     <row r="22" spans="2:19">
       <c r="B22" s="16" t="s">
-        <v>51</v>
-      </c>
-      <c r="C22" s="5"/>
+        <v>30</v>
+      </c>
+      <c r="C22" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="D22" t="b">
+        <v>1</v>
+      </c>
       <c r="E22" t="b">
         <v>1</v>
       </c>
@@ -1546,90 +1529,97 @@
       <c r="G22" t="b">
         <v>1</v>
       </c>
+      <c r="H22" t="b">
+        <v>1</v>
+      </c>
       <c r="I22" t="b">
         <v>1</v>
       </c>
+      <c r="K22" t="b">
+        <v>1</v>
+      </c>
       <c r="L22" t="b">
         <v>1</v>
       </c>
       <c r="M22" t="b">
         <v>1</v>
       </c>
+      <c r="N22" t="b">
+        <v>1</v>
+      </c>
       <c r="P22" s="9" t="b">
         <v>1</v>
       </c>
       <c r="Q22" s="10">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="R22" s="13" t="s">
         <v>68</v>
       </c>
       <c r="S22" s="14">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="23" spans="2:19">
       <c r="B23" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="C23" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="D23" t="b">
-        <v>1</v>
-      </c>
-      <c r="E23" t="b">
-        <v>1</v>
-      </c>
-      <c r="F23" t="b">
-        <v>1</v>
-      </c>
-      <c r="H23" t="b">
-        <v>1</v>
-      </c>
-      <c r="K23" t="b">
-        <v>1</v>
-      </c>
-      <c r="N23" t="b">
-        <v>1</v>
-      </c>
-      <c r="O23" t="b">
-        <v>1</v>
-      </c>
-      <c r="P23" s="9"/>
+        <v>72</v>
+      </c>
+      <c r="C23" s="5"/>
+      <c r="P23" s="9" t="b">
+        <v>1</v>
+      </c>
       <c r="Q23" s="10">
         <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="R23" s="13" t="s">
-        <v>67</v>
-      </c>
-      <c r="S23" s="14">
-        <v>10</v>
+        <v>1</v>
+      </c>
+      <c r="R23" s="20" t="s">
+        <v>68</v>
+      </c>
+      <c r="S23" s="21">
+        <v>7</v>
       </c>
     </row>
     <row r="24" spans="2:19">
       <c r="B24" s="16" t="s">
-        <v>41</v>
+        <v>51</v>
       </c>
       <c r="C24" s="5"/>
-      <c r="D24" t="b">
-        <v>1</v>
-      </c>
-      <c r="P24" s="9"/>
+      <c r="E24" t="b">
+        <v>1</v>
+      </c>
+      <c r="F24" t="b">
+        <v>1</v>
+      </c>
+      <c r="G24" t="b">
+        <v>1</v>
+      </c>
+      <c r="I24" t="b">
+        <v>1</v>
+      </c>
+      <c r="L24" t="b">
+        <v>1</v>
+      </c>
+      <c r="M24" t="b">
+        <v>1</v>
+      </c>
+      <c r="P24" s="9" t="b">
+        <v>1</v>
+      </c>
       <c r="Q24" s="10">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="R24" s="13"/>
+        <v>7</v>
+      </c>
+      <c r="R24" s="13" t="s">
+        <v>68</v>
+      </c>
       <c r="S24" s="14">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="25" spans="2:19">
       <c r="B25" s="16" t="s">
-        <v>19</v>
+        <v>34</v>
       </c>
       <c r="C25" s="5" t="b">
         <v>1</v>
@@ -1640,7 +1630,13 @@
       <c r="E25" t="b">
         <v>1</v>
       </c>
-      <c r="M25" t="b">
+      <c r="F25" t="b">
+        <v>1</v>
+      </c>
+      <c r="H25" t="b">
+        <v>1</v>
+      </c>
+      <c r="K25" t="b">
         <v>1</v>
       </c>
       <c r="N25" t="b">
@@ -1649,15 +1645,13 @@
       <c r="O25" t="b">
         <v>1</v>
       </c>
-      <c r="P25" s="9" t="b">
-        <v>1</v>
-      </c>
+      <c r="P25" s="9"/>
       <c r="Q25" s="10">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="R25" s="13" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="S25" s="14">
         <v>10</v>
@@ -1665,54 +1659,35 @@
     </row>
     <row r="26" spans="2:19">
       <c r="B26" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="C26" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="O26" t="b">
-        <v>1</v>
-      </c>
-      <c r="P26" s="9" t="b">
-        <v>1</v>
-      </c>
+        <v>41</v>
+      </c>
+      <c r="C26" s="5"/>
+      <c r="D26" t="b">
+        <v>1</v>
+      </c>
+      <c r="P26" s="9"/>
       <c r="Q26" s="10">
         <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="R26" s="13" t="s">
-        <v>68</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="R26" s="13"/>
       <c r="S26" s="14">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="27" spans="2:19">
       <c r="B27" s="16" t="s">
-        <v>37</v>
-      </c>
-      <c r="C27" s="5"/>
+        <v>19</v>
+      </c>
+      <c r="C27" s="5" t="b">
+        <v>1</v>
+      </c>
       <c r="D27" t="b">
         <v>1</v>
       </c>
       <c r="E27" t="b">
         <v>1</v>
       </c>
-      <c r="F27" t="b">
-        <v>1</v>
-      </c>
-      <c r="G27" t="b">
-        <v>1</v>
-      </c>
-      <c r="H27" t="b">
-        <v>1</v>
-      </c>
-      <c r="I27" t="b">
-        <v>1</v>
-      </c>
-      <c r="J27" t="b">
-        <v>1</v>
-      </c>
       <c r="M27" t="b">
         <v>1</v>
       </c>
@@ -1722,56 +1697,27 @@
       <c r="O27" t="b">
         <v>1</v>
       </c>
-      <c r="P27" s="9"/>
+      <c r="P27" s="9" t="b">
+        <v>1</v>
+      </c>
       <c r="Q27" s="10">
         <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="R27" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="S27" s="14">
         <v>10</v>
-      </c>
-      <c r="R27" s="13"/>
-      <c r="S27" s="14">
-        <v>6</v>
       </c>
     </row>
     <row r="28" spans="2:19">
       <c r="B28" s="16" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C28" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="D28" t="b">
-        <v>1</v>
-      </c>
-      <c r="E28" t="b">
-        <v>1</v>
-      </c>
-      <c r="F28" t="b">
-        <v>1</v>
-      </c>
-      <c r="G28" t="b">
-        <v>1</v>
-      </c>
-      <c r="H28" t="b">
-        <v>1</v>
-      </c>
-      <c r="I28" t="b">
-        <v>1</v>
-      </c>
-      <c r="J28" t="b">
-        <v>1</v>
-      </c>
-      <c r="K28" t="b">
-        <v>1</v>
-      </c>
-      <c r="L28" t="b">
-        <v>1</v>
-      </c>
-      <c r="M28" t="b">
-        <v>1</v>
-      </c>
-      <c r="N28" t="b">
-        <v>1</v>
-      </c>
       <c r="O28" t="b">
         <v>1</v>
       </c>
@@ -1780,18 +1726,18 @@
       </c>
       <c r="Q28" s="10">
         <f t="shared" si="0"/>
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="R28" s="13" t="s">
         <v>68</v>
       </c>
       <c r="S28" s="14">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="29" spans="2:19">
       <c r="B29" s="16" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="C29" s="5"/>
       <c r="D29" t="b">
@@ -1800,6 +1746,9 @@
       <c r="E29" t="b">
         <v>1</v>
       </c>
+      <c r="F29" t="b">
+        <v>1</v>
+      </c>
       <c r="G29" t="b">
         <v>1</v>
       </c>
@@ -1812,29 +1761,28 @@
       <c r="J29" t="b">
         <v>1</v>
       </c>
-      <c r="K29" t="b">
+      <c r="M29" t="b">
+        <v>1</v>
+      </c>
+      <c r="N29" t="b">
         <v>1</v>
       </c>
       <c r="O29" t="b">
         <v>1</v>
       </c>
-      <c r="P29" s="9" t="b">
-        <v>1</v>
-      </c>
+      <c r="P29" s="9"/>
       <c r="Q29" s="10">
         <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
-      <c r="R29" s="13" t="s">
-        <v>68</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="R29" s="13"/>
       <c r="S29" s="14">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="30" spans="2:19">
       <c r="B30" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C30" s="5" t="b">
         <v>1</v>
@@ -1863,32 +1811,46 @@
       <c r="K30" t="b">
         <v>1</v>
       </c>
+      <c r="L30" t="b">
+        <v>1</v>
+      </c>
+      <c r="M30" t="b">
+        <v>1</v>
+      </c>
       <c r="N30" t="b">
         <v>1</v>
       </c>
       <c r="O30" t="b">
         <v>1</v>
       </c>
-      <c r="P30" s="9"/>
+      <c r="P30" s="9" t="b">
+        <v>1</v>
+      </c>
       <c r="Q30" s="10">
         <f t="shared" si="0"/>
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="R30" s="13" t="s">
         <v>68</v>
       </c>
       <c r="S30" s="14">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="31" spans="2:19">
       <c r="B31" s="16" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C31" s="5"/>
       <c r="D31" t="b">
         <v>1</v>
       </c>
+      <c r="E31" t="b">
+        <v>1</v>
+      </c>
+      <c r="G31" t="b">
+        <v>1</v>
+      </c>
       <c r="H31" t="b">
         <v>1</v>
       </c>
@@ -1901,65 +1863,105 @@
       <c r="K31" t="b">
         <v>1</v>
       </c>
-      <c r="M31" t="b">
-        <v>1</v>
-      </c>
       <c r="O31" t="b">
         <v>1</v>
       </c>
-      <c r="P31" s="9"/>
+      <c r="P31" s="9" t="b">
+        <v>1</v>
+      </c>
       <c r="Q31" s="10">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="R31" s="13" t="s">
         <v>68</v>
       </c>
       <c r="S31" s="14">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="32" spans="2:19">
       <c r="B32" s="16" t="s">
-        <v>36</v>
-      </c>
-      <c r="C32" s="5"/>
+        <v>22</v>
+      </c>
+      <c r="C32" s="5" t="b">
+        <v>1</v>
+      </c>
       <c r="D32" t="b">
+        <v>1</v>
+      </c>
+      <c r="E32" t="b">
+        <v>1</v>
+      </c>
+      <c r="F32" t="b">
+        <v>1</v>
+      </c>
+      <c r="G32" t="b">
+        <v>1</v>
+      </c>
+      <c r="H32" t="b">
+        <v>1</v>
+      </c>
+      <c r="I32" t="b">
+        <v>1</v>
+      </c>
+      <c r="J32" t="b">
+        <v>1</v>
+      </c>
+      <c r="K32" t="b">
+        <v>1</v>
+      </c>
+      <c r="N32" t="b">
+        <v>1</v>
+      </c>
+      <c r="O32" t="b">
         <v>1</v>
       </c>
       <c r="P32" s="9"/>
       <c r="Q32" s="10">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="R32" s="13"/>
+        <v>11</v>
+      </c>
+      <c r="R32" s="13" t="s">
+        <v>68</v>
+      </c>
       <c r="S32" s="14">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="33" spans="2:19">
       <c r="B33" s="16" t="s">
-        <v>62</v>
+        <v>44</v>
       </c>
       <c r="C33" s="5"/>
+      <c r="D33" t="b">
+        <v>1</v>
+      </c>
+      <c r="H33" t="b">
+        <v>1</v>
+      </c>
+      <c r="I33" t="b">
+        <v>1</v>
+      </c>
+      <c r="J33" t="b">
+        <v>1</v>
+      </c>
       <c r="K33" t="b">
         <v>1</v>
       </c>
-      <c r="N33" t="b">
+      <c r="M33" t="b">
         <v>1</v>
       </c>
       <c r="O33" t="b">
         <v>1</v>
       </c>
-      <c r="P33" s="9" t="b">
-        <v>1</v>
-      </c>
+      <c r="P33" s="9"/>
       <c r="Q33" s="10">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="R33" s="13" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="S33" s="14">
         <v>10</v>
@@ -1967,49 +1969,28 @@
     </row>
     <row r="34" spans="2:19">
       <c r="B34" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="C34" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="E34" t="b">
-        <v>1</v>
-      </c>
-      <c r="F34" t="b">
-        <v>1</v>
-      </c>
-      <c r="I34" t="b">
-        <v>1</v>
-      </c>
-      <c r="O34" t="b">
-        <v>1</v>
-      </c>
-      <c r="P34" s="9" t="b">
-        <v>1</v>
-      </c>
+        <v>36</v>
+      </c>
+      <c r="C34" s="5"/>
+      <c r="D34" t="b">
+        <v>1</v>
+      </c>
+      <c r="P34" s="9"/>
       <c r="Q34" s="10">
         <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="R34" s="13" t="s">
-        <v>74</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="R34" s="13"/>
       <c r="S34" s="14">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="35" spans="2:19">
       <c r="B35" s="16" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="C35" s="5"/>
-      <c r="H35" t="b">
-        <v>1</v>
-      </c>
-      <c r="I35" t="b">
-        <v>1</v>
-      </c>
-      <c r="M35" t="b">
+      <c r="K35" t="b">
         <v>1</v>
       </c>
       <c r="N35" t="b">
@@ -2018,107 +1999,64 @@
       <c r="O35" t="b">
         <v>1</v>
       </c>
-      <c r="P35" s="9"/>
+      <c r="P35" s="9" t="b">
+        <v>1</v>
+      </c>
       <c r="Q35" s="10">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="R35" s="13" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="S35" s="14">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="36" spans="2:19">
       <c r="B36" s="16" t="s">
-        <v>23</v>
+        <v>35</v>
       </c>
       <c r="C36" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="D36" t="b">
-        <v>1</v>
-      </c>
       <c r="E36" t="b">
         <v>1</v>
       </c>
       <c r="F36" t="b">
         <v>1</v>
       </c>
-      <c r="G36" t="b">
-        <v>1</v>
-      </c>
-      <c r="H36" t="b">
-        <v>1</v>
-      </c>
       <c r="I36" t="b">
         <v>1</v>
       </c>
-      <c r="J36" t="b">
-        <v>1</v>
-      </c>
-      <c r="K36" t="b">
-        <v>1</v>
-      </c>
-      <c r="L36" t="b">
-        <v>1</v>
-      </c>
-      <c r="M36" t="b">
-        <v>1</v>
-      </c>
-      <c r="N36" t="b">
-        <v>1</v>
-      </c>
       <c r="O36" t="b">
         <v>1</v>
       </c>
-      <c r="P36" s="9"/>
+      <c r="P36" s="9" t="b">
+        <v>1</v>
+      </c>
       <c r="Q36" s="10">
         <f t="shared" si="0"/>
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="R36" s="13" t="s">
-        <v>63</v>
+        <v>74</v>
       </c>
       <c r="S36" s="14">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="37" spans="2:19">
       <c r="B37" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="C37" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="D37" t="b">
-        <v>1</v>
-      </c>
-      <c r="E37" t="b">
-        <v>1</v>
-      </c>
-      <c r="F37" t="b">
-        <v>1</v>
-      </c>
-      <c r="G37" t="b">
-        <v>1</v>
-      </c>
+        <v>58</v>
+      </c>
+      <c r="C37" s="5"/>
       <c r="H37" t="b">
         <v>1</v>
       </c>
       <c r="I37" t="b">
         <v>1</v>
       </c>
-      <c r="J37" t="b">
-        <v>1</v>
-      </c>
-      <c r="K37" t="b">
-        <v>1</v>
-      </c>
-      <c r="L37" t="b">
-        <v>1</v>
-      </c>
       <c r="M37" t="b">
         <v>1</v>
       </c>
@@ -2128,53 +2066,83 @@
       <c r="O37" t="b">
         <v>1</v>
       </c>
-      <c r="P37" s="9" t="b">
-        <v>1</v>
-      </c>
+      <c r="P37" s="9"/>
       <c r="Q37" s="10">
         <f t="shared" si="0"/>
-        <v>14</v>
-      </c>
-      <c r="R37" s="13"/>
+        <v>5</v>
+      </c>
+      <c r="R37" s="13" t="s">
+        <v>68</v>
+      </c>
       <c r="S37" s="14">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="38" spans="2:19">
       <c r="B38" s="16" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C38" s="5" t="b">
         <v>1</v>
       </c>
+      <c r="D38" t="b">
+        <v>1</v>
+      </c>
+      <c r="E38" t="b">
+        <v>1</v>
+      </c>
+      <c r="F38" t="b">
+        <v>1</v>
+      </c>
       <c r="G38" t="b">
         <v>1</v>
       </c>
+      <c r="H38" t="b">
+        <v>1</v>
+      </c>
+      <c r="I38" t="b">
+        <v>1</v>
+      </c>
+      <c r="J38" t="b">
+        <v>1</v>
+      </c>
       <c r="K38" t="b">
         <v>1</v>
       </c>
+      <c r="L38" t="b">
+        <v>1</v>
+      </c>
+      <c r="M38" t="b">
+        <v>1</v>
+      </c>
       <c r="N38" t="b">
         <v>1</v>
       </c>
-      <c r="P38" s="9" t="b">
-        <v>1</v>
-      </c>
+      <c r="O38" t="b">
+        <v>1</v>
+      </c>
+      <c r="P38" s="9"/>
       <c r="Q38" s="10">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="R38" s="13" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="S38" s="14">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="39" spans="2:19">
       <c r="B39" s="16" t="s">
-        <v>52</v>
-      </c>
-      <c r="C39" s="5"/>
+        <v>24</v>
+      </c>
+      <c r="C39" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="D39" t="b">
+        <v>1</v>
+      </c>
       <c r="E39" t="b">
         <v>1</v>
       </c>
@@ -2184,25 +2152,39 @@
       <c r="G39" t="b">
         <v>1</v>
       </c>
+      <c r="H39" t="b">
+        <v>1</v>
+      </c>
       <c r="I39" t="b">
         <v>1</v>
       </c>
       <c r="J39" t="b">
         <v>1</v>
       </c>
+      <c r="K39" t="b">
+        <v>1</v>
+      </c>
+      <c r="L39" t="b">
+        <v>1</v>
+      </c>
       <c r="M39" t="b">
         <v>1</v>
       </c>
+      <c r="N39" t="b">
+        <v>1</v>
+      </c>
       <c r="O39" t="b">
         <v>1</v>
       </c>
-      <c r="P39" s="9"/>
+      <c r="P39" s="9" t="b">
+        <v>1</v>
+      </c>
       <c r="Q39" s="10">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="R39" s="13" t="s">
-        <v>68</v>
+        <v>79</v>
       </c>
       <c r="S39" s="14">
         <v>10</v>
@@ -2210,27 +2192,18 @@
     </row>
     <row r="40" spans="2:19">
       <c r="B40" s="16" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C40" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="D40" t="b">
-        <v>1</v>
-      </c>
-      <c r="E40" t="b">
-        <v>1</v>
-      </c>
-      <c r="F40" t="b">
-        <v>1</v>
-      </c>
       <c r="G40" t="b">
         <v>1</v>
       </c>
-      <c r="I40" t="b">
-        <v>1</v>
-      </c>
-      <c r="J40" t="b">
+      <c r="K40" t="b">
+        <v>1</v>
+      </c>
+      <c r="N40" t="b">
         <v>1</v>
       </c>
       <c r="P40" s="9" t="b">
@@ -2238,10 +2211,10 @@
       </c>
       <c r="Q40" s="10">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="R40" s="13" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="S40" s="14">
         <v>9</v>
@@ -2249,60 +2222,65 @@
     </row>
     <row r="41" spans="2:19">
       <c r="B41" s="16" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C41" s="5"/>
       <c r="E41" t="b">
         <v>1</v>
       </c>
+      <c r="F41" t="b">
+        <v>1</v>
+      </c>
+      <c r="G41" t="b">
+        <v>1</v>
+      </c>
+      <c r="I41" t="b">
+        <v>1</v>
+      </c>
+      <c r="J41" t="b">
+        <v>1</v>
+      </c>
       <c r="M41" t="b">
         <v>1</v>
       </c>
-      <c r="N41" t="b">
-        <v>1</v>
-      </c>
       <c r="O41" t="b">
         <v>1</v>
       </c>
-      <c r="P41" s="9" t="b">
-        <v>1</v>
-      </c>
+      <c r="P41" s="9"/>
       <c r="Q41" s="10">
         <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="R41" s="13"/>
+        <v>7</v>
+      </c>
+      <c r="R41" s="13" t="s">
+        <v>68</v>
+      </c>
       <c r="S41" s="14">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="42" spans="2:19">
       <c r="B42" s="16" t="s">
-        <v>40</v>
-      </c>
-      <c r="C42" s="5"/>
+        <v>26</v>
+      </c>
+      <c r="C42" s="5" t="b">
+        <v>1</v>
+      </c>
       <c r="D42" t="b">
         <v>1</v>
       </c>
       <c r="E42" t="b">
         <v>1</v>
       </c>
+      <c r="F42" t="b">
+        <v>1</v>
+      </c>
       <c r="G42" t="b">
         <v>1</v>
       </c>
-      <c r="H42" t="b">
-        <v>1</v>
-      </c>
       <c r="I42" t="b">
         <v>1</v>
       </c>
-      <c r="L42" t="b">
-        <v>1</v>
-      </c>
-      <c r="M42" t="b">
-        <v>1</v>
-      </c>
-      <c r="O42" t="b">
+      <c r="J42" t="b">
         <v>1</v>
       </c>
       <c r="P42" s="9" t="b">
@@ -2310,44 +2288,55 @@
       </c>
       <c r="Q42" s="10">
         <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="R42" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="S42" s="14">
         <v>9</v>
-      </c>
-      <c r="R42" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="S42" s="14">
-        <v>8</v>
       </c>
     </row>
     <row r="43" spans="2:19">
       <c r="B43" s="16" t="s">
-        <v>61</v>
+        <v>48</v>
       </c>
       <c r="C43" s="5"/>
-      <c r="J43" t="b">
+      <c r="E43" t="b">
         <v>1</v>
       </c>
       <c r="M43" t="b">
         <v>1</v>
       </c>
+      <c r="N43" t="b">
+        <v>1</v>
+      </c>
       <c r="O43" t="b">
         <v>1</v>
       </c>
-      <c r="P43" s="9"/>
+      <c r="P43" s="9" t="b">
+        <v>1</v>
+      </c>
       <c r="Q43" s="10">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="R43" s="13"/>
       <c r="S43" s="14">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="44" spans="2:19">
       <c r="B44" s="17" t="s">
-        <v>55</v>
+        <v>40</v>
       </c>
       <c r="C44" s="5"/>
+      <c r="D44" t="b">
+        <v>1</v>
+      </c>
+      <c r="E44" t="b">
+        <v>1</v>
+      </c>
       <c r="G44" t="b">
         <v>1</v>
       </c>
@@ -2357,7 +2346,7 @@
       <c r="I44" t="b">
         <v>1</v>
       </c>
-      <c r="J44" t="b">
+      <c r="L44" t="b">
         <v>1</v>
       </c>
       <c r="M44" t="b">
@@ -2371,36 +2360,21 @@
       </c>
       <c r="Q44" s="10">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="R44" s="13" t="s">
         <v>68</v>
       </c>
       <c r="S44" s="14">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="45" spans="2:19">
       <c r="B45" s="16" t="s">
-        <v>42</v>
+        <v>61</v>
       </c>
       <c r="C45" s="5"/>
-      <c r="D45" t="b">
-        <v>1</v>
-      </c>
-      <c r="E45" t="b">
-        <v>1</v>
-      </c>
-      <c r="F45" t="b">
-        <v>1</v>
-      </c>
-      <c r="G45" t="b">
-        <v>1</v>
-      </c>
-      <c r="H45" t="b">
-        <v>1</v>
-      </c>
-      <c r="I45" t="b">
+      <c r="J45" t="b">
         <v>1</v>
       </c>
       <c r="M45" t="b">
@@ -2412,136 +2386,195 @@
       <c r="P45" s="9"/>
       <c r="Q45" s="10">
         <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="R45" s="13" t="s">
-        <v>68</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="R45" s="13"/>
       <c r="S45" s="14">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="46" spans="2:19">
       <c r="B46" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="C46" s="5"/>
+      <c r="G46" t="b">
+        <v>1</v>
+      </c>
+      <c r="H46" t="b">
+        <v>1</v>
+      </c>
+      <c r="I46" t="b">
+        <v>1</v>
+      </c>
+      <c r="J46" t="b">
+        <v>1</v>
+      </c>
+      <c r="M46" t="b">
+        <v>1</v>
+      </c>
+      <c r="O46" t="b">
+        <v>1</v>
+      </c>
+      <c r="P46" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q46" s="10">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="R46" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="S46" s="14">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="47" spans="2:19">
+      <c r="B47" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="C47" s="5"/>
+      <c r="D47" t="b">
+        <v>1</v>
+      </c>
+      <c r="E47" t="b">
+        <v>1</v>
+      </c>
+      <c r="F47" t="b">
+        <v>1</v>
+      </c>
+      <c r="G47" t="b">
+        <v>1</v>
+      </c>
+      <c r="H47" t="b">
+        <v>1</v>
+      </c>
+      <c r="I47" t="b">
+        <v>1</v>
+      </c>
+      <c r="M47" t="b">
+        <v>1</v>
+      </c>
+      <c r="O47" t="b">
+        <v>1</v>
+      </c>
+      <c r="P47" s="9"/>
+      <c r="Q47" s="10">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="R47" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="S47" s="14">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="48" spans="2:19">
+      <c r="B48" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="C46" s="5"/>
-      <c r="F46" t="b">
-        <v>1</v>
-      </c>
-      <c r="G46" t="b">
-        <v>1</v>
-      </c>
-      <c r="I46" t="b">
-        <v>1</v>
-      </c>
-      <c r="K46" t="b">
-        <v>1</v>
-      </c>
-      <c r="L46" t="b">
-        <v>1</v>
-      </c>
-      <c r="M46" t="b">
-        <v>1</v>
-      </c>
-      <c r="P46" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q46" s="10">
+      <c r="C48" s="5"/>
+      <c r="F48" t="b">
+        <v>1</v>
+      </c>
+      <c r="G48" t="b">
+        <v>1</v>
+      </c>
+      <c r="I48" t="b">
+        <v>1</v>
+      </c>
+      <c r="K48" t="b">
+        <v>1</v>
+      </c>
+      <c r="L48" t="b">
+        <v>1</v>
+      </c>
+      <c r="M48" t="b">
+        <v>1</v>
+      </c>
+      <c r="P48" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q48" s="10">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="R46" s="13" t="s">
+      <c r="R48" s="13" t="s">
         <v>73</v>
       </c>
-      <c r="S46" s="14">
+      <c r="S48" s="14">
         <v>10</v>
       </c>
     </row>
-    <row r="47" spans="2:19">
-      <c r="B47" s="16" t="s">
+    <row r="49" spans="2:19">
+      <c r="B49" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="C49" s="5"/>
+      <c r="P49" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q49" s="10">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="R49" s="20" t="s">
+        <v>68</v>
+      </c>
+      <c r="S49" s="14">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="50" spans="2:19">
+      <c r="B50" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="C47" s="6"/>
-      <c r="D47" s="7"/>
-      <c r="E47" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="F47" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="G47" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="H47" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="I47" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="J47" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="K47" s="7"/>
-      <c r="L47" s="7"/>
-      <c r="M47" s="7"/>
-      <c r="N47" s="7"/>
-      <c r="O47" s="7"/>
-      <c r="P47" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q47" s="18">
+      <c r="C50" s="6"/>
+      <c r="D50" s="7"/>
+      <c r="E50" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F50" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="G50" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="H50" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="I50" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="J50" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="K50" s="7"/>
+      <c r="L50" s="7"/>
+      <c r="M50" s="7"/>
+      <c r="N50" s="7"/>
+      <c r="O50" s="7"/>
+      <c r="P50" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q50" s="10">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="R47" s="19" t="s">
+      <c r="R50" s="22" t="s">
         <v>76</v>
       </c>
-      <c r="S47" s="15">
+      <c r="S50" s="15">
         <v>9</v>
       </c>
     </row>
-    <row r="48" spans="2:19">
-      <c r="B48" s="16" t="s">
-        <v>71</v>
-      </c>
-      <c r="P48" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q48" s="18">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="R48" t="s">
-        <v>68</v>
-      </c>
-      <c r="S48" s="20">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="49" spans="2:19">
-      <c r="B49" s="16" t="s">
-        <v>72</v>
-      </c>
-      <c r="P49" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q49" s="18">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="R49" t="s">
-        <v>68</v>
-      </c>
-      <c r="S49">
-        <v>7</v>
-      </c>
-    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:S47">
-    <sortCondition ref="B47"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:S50">
+    <sortCondition ref="B3:B50"/>
   </sortState>
-  <conditionalFormatting sqref="Q3:Q49">
+  <conditionalFormatting sqref="Q3:Q50">
     <cfRule type="cellIs" dxfId="0" priority="2" operator="lessThan">
       <formula>4</formula>
     </cfRule>

</xml_diff>